<commit_message>
Update TX data for today/now (2020-06-24T02:48:56Z)
</commit_message>
<xml_diff>
--- a/raw/TX/TexasCOVID-19CumulativeTestsOverTimebyCounty.xlsx
+++ b/raw/TX/TexasCOVID-19CumulativeTestsOverTimebyCounty.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F1C9568C-DA55-434B-91A1-F38EF27839C9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1430C315-D6B2-439C-8E8F-4EB7CE9ECA2A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="331">
   <si>
     <t>County</t>
   </si>
@@ -1019,7 +1019,10 @@
     <t>Tests Through June 21</t>
   </si>
   <si>
-    <t>5. This file will be updated daily; the next cumulative update will be 6/23/2020.</t>
+    <t>Tests Through June 22</t>
+  </si>
+  <si>
+    <t>5. This file will be updated daily; the next cumulative update will be 6/24/2020.</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK267"/>
+  <dimension ref="A1:BL267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -1478,15 +1481,15 @@
     <col min="46" max="46" width="11.453125" style="2" customWidth="1"/>
     <col min="47" max="49" width="11.1796875" style="2" customWidth="1"/>
     <col min="50" max="59" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="63" width="12.90625" customWidth="1"/>
+    <col min="60" max="64" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:64" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1676,8 +1679,11 @@
       <c r="BK2" s="7" t="s">
         <v>328</v>
       </c>
+      <c r="BL2" s="7" t="s">
+        <v>329</v>
+      </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1867,8 +1873,11 @@
       <c r="BK3" s="2">
         <v>3309</v>
       </c>
+      <c r="BL3" s="2">
+        <v>5058</v>
+      </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2058,8 +2067,11 @@
       <c r="BK4" s="2">
         <v>91</v>
       </c>
+      <c r="BL4" s="2">
+        <v>95</v>
+      </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2249,8 +2261,11 @@
       <c r="BK5" s="2">
         <v>3599</v>
       </c>
+      <c r="BL5" s="2">
+        <v>3662</v>
+      </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2440,8 +2455,11 @@
       <c r="BK6" s="2">
         <v>337</v>
       </c>
+      <c r="BL6" s="2">
+        <v>342</v>
+      </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2631,8 +2649,11 @@
       <c r="BK7" s="2">
         <v>89</v>
       </c>
+      <c r="BL7" s="2">
+        <v>94</v>
+      </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2822,8 +2843,11 @@
       <c r="BK8" s="2">
         <v>178</v>
       </c>
+      <c r="BL8" s="2">
+        <v>180</v>
+      </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -3013,8 +3037,11 @@
       <c r="BK9" s="2">
         <v>1406</v>
       </c>
+      <c r="BL9" s="2">
+        <v>1424</v>
+      </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -3204,8 +3231,11 @@
       <c r="BK10" s="2">
         <v>1402</v>
       </c>
+      <c r="BL10" s="2">
+        <v>1418</v>
+      </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -3395,8 +3425,11 @@
       <c r="BK11" s="2">
         <v>107</v>
       </c>
+      <c r="BL11" s="2">
+        <v>107</v>
+      </c>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -3586,8 +3619,11 @@
       <c r="BK12" s="2">
         <v>414</v>
       </c>
+      <c r="BL12" s="2">
+        <v>425</v>
+      </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -3777,8 +3813,11 @@
       <c r="BK13" s="2">
         <v>2225</v>
       </c>
+      <c r="BL13" s="2">
+        <v>2285</v>
+      </c>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -3968,8 +4007,11 @@
       <c r="BK14" s="2">
         <v>73</v>
       </c>
+      <c r="BL14" s="2">
+        <v>73</v>
+      </c>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -4159,8 +4201,11 @@
       <c r="BK15" s="2">
         <v>1144</v>
       </c>
+      <c r="BL15" s="2">
+        <v>1734</v>
+      </c>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -4350,8 +4395,11 @@
       <c r="BK16" s="2">
         <v>22219</v>
       </c>
+      <c r="BL16" s="2">
+        <v>22592</v>
+      </c>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -4541,8 +4589,11 @@
       <c r="BK17" s="2">
         <v>62316</v>
       </c>
+      <c r="BL17" s="2">
+        <v>63752</v>
+      </c>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -4732,8 +4783,11 @@
       <c r="BK18" s="2">
         <v>2006</v>
       </c>
+      <c r="BL18" s="2">
+        <v>2044</v>
+      </c>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -4923,8 +4977,11 @@
       <c r="BK19" s="2">
         <v>2</v>
       </c>
+      <c r="BL19" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -5114,8 +5171,11 @@
       <c r="BK20" s="2">
         <v>992</v>
       </c>
+      <c r="BL20" s="2">
+        <v>998</v>
+      </c>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -5305,8 +5365,11 @@
       <c r="BK21" s="2">
         <v>4568</v>
       </c>
+      <c r="BL21" s="2">
+        <v>6910</v>
+      </c>
     </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -5496,8 +5559,11 @@
       <c r="BK22" s="2">
         <v>13889</v>
       </c>
+      <c r="BL22" s="2">
+        <v>14138</v>
+      </c>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
@@ -5687,8 +5753,11 @@
       <c r="BK23" s="2">
         <v>12096</v>
       </c>
+      <c r="BL23" s="2">
+        <v>12295</v>
+      </c>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -5878,8 +5947,11 @@
       <c r="BK24" s="2">
         <v>658</v>
       </c>
+      <c r="BL24" s="2">
+        <v>943</v>
+      </c>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
@@ -6069,8 +6141,11 @@
       <c r="BK25" s="2">
         <v>53</v>
       </c>
+      <c r="BL25" s="2">
+        <v>56</v>
+      </c>
     </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -6260,8 +6335,11 @@
       <c r="BK26" s="2">
         <v>98</v>
       </c>
+      <c r="BL26" s="2">
+        <v>111</v>
+      </c>
     </row>
-    <row r="27" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -6451,8 +6529,11 @@
       <c r="BK27" s="2">
         <v>1029</v>
       </c>
+      <c r="BL27" s="2">
+        <v>1061</v>
+      </c>
     </row>
-    <row r="28" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -6642,8 +6723,11 @@
       <c r="BK28" s="2">
         <v>689</v>
       </c>
+      <c r="BL28" s="2">
+        <v>703</v>
+      </c>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
@@ -6833,8 +6917,11 @@
       <c r="BK29" s="2">
         <v>1734</v>
       </c>
+      <c r="BL29" s="2">
+        <v>1752</v>
+      </c>
     </row>
-    <row r="30" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -7024,8 +7111,11 @@
       <c r="BK30" s="2">
         <v>1097</v>
       </c>
+      <c r="BL30" s="2">
+        <v>1145</v>
+      </c>
     </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -7215,8 +7305,11 @@
       <c r="BK31" s="2">
         <v>1013</v>
       </c>
+      <c r="BL31" s="2">
+        <v>1013</v>
+      </c>
     </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>30</v>
       </c>
@@ -7406,8 +7499,11 @@
       <c r="BK32" s="2">
         <v>305</v>
       </c>
+      <c r="BL32" s="2">
+        <v>315</v>
+      </c>
     </row>
-    <row r="33" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
@@ -7597,8 +7693,11 @@
       <c r="BK33" s="2">
         <v>13358</v>
       </c>
+      <c r="BL33" s="2">
+        <v>13833</v>
+      </c>
     </row>
-    <row r="34" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
@@ -7788,8 +7887,11 @@
       <c r="BK34" s="2">
         <v>351</v>
       </c>
+      <c r="BL34" s="2">
+        <v>356</v>
+      </c>
     </row>
-    <row r="35" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>33</v>
       </c>
@@ -7979,8 +8081,11 @@
       <c r="BK35" s="2">
         <v>149</v>
       </c>
+      <c r="BL35" s="2">
+        <v>152</v>
+      </c>
     </row>
-    <row r="36" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>34</v>
       </c>
@@ -8170,8 +8275,11 @@
       <c r="BK36" s="2">
         <v>750</v>
       </c>
+      <c r="BL36" s="2">
+        <v>778</v>
+      </c>
     </row>
-    <row r="37" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
@@ -8361,8 +8469,11 @@
       <c r="BK37" s="2">
         <v>317</v>
       </c>
+      <c r="BL37" s="2">
+        <v>318</v>
+      </c>
     </row>
-    <row r="38" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>36</v>
       </c>
@@ -8552,8 +8663,11 @@
       <c r="BK38" s="2">
         <v>1426</v>
       </c>
+      <c r="BL38" s="2">
+        <v>1441</v>
+      </c>
     </row>
-    <row r="39" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
@@ -8743,8 +8857,11 @@
       <c r="BK39" s="2">
         <v>1319</v>
       </c>
+      <c r="BL39" s="2">
+        <v>1392</v>
+      </c>
     </row>
-    <row r="40" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>38</v>
       </c>
@@ -8934,8 +9051,11 @@
       <c r="BK40" s="2">
         <v>281</v>
       </c>
+      <c r="BL40" s="2">
+        <v>289</v>
+      </c>
     </row>
-    <row r="41" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
@@ -9125,8 +9245,11 @@
       <c r="BK41" s="2">
         <v>318</v>
       </c>
+      <c r="BL41" s="2">
+        <v>325</v>
+      </c>
     </row>
-    <row r="42" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
@@ -9316,8 +9439,11 @@
       <c r="BK42" s="2">
         <v>19</v>
       </c>
+      <c r="BL42" s="2">
+        <v>19</v>
+      </c>
     </row>
-    <row r="43" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>41</v>
       </c>
@@ -9507,8 +9633,11 @@
       <c r="BK43" s="2">
         <v>36</v>
       </c>
+      <c r="BL43" s="2">
+        <v>36</v>
+      </c>
     </row>
-    <row r="44" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
@@ -9698,8 +9827,11 @@
       <c r="BK44" s="2">
         <v>188</v>
       </c>
+      <c r="BL44" s="2">
+        <v>190</v>
+      </c>
     </row>
-    <row r="45" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
@@ -9889,8 +10021,11 @@
       <c r="BK45" s="2">
         <v>38626</v>
       </c>
+      <c r="BL45" s="2">
+        <v>39489</v>
+      </c>
     </row>
-    <row r="46" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>44</v>
       </c>
@@ -10080,8 +10215,11 @@
       <c r="BK46" s="2">
         <v>157</v>
       </c>
+      <c r="BL46" s="2">
+        <v>159</v>
+      </c>
     </row>
-    <row r="47" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
@@ -10271,8 +10409,11 @@
       <c r="BK47" s="2">
         <v>1134</v>
       </c>
+      <c r="BL47" s="2">
+        <v>1183</v>
+      </c>
     </row>
-    <row r="48" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>46</v>
       </c>
@@ -10462,8 +10603,11 @@
       <c r="BK48" s="2">
         <v>5191</v>
       </c>
+      <c r="BL48" s="2">
+        <v>5302</v>
+      </c>
     </row>
-    <row r="49" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
@@ -10653,8 +10797,11 @@
       <c r="BK49" s="2">
         <v>673</v>
       </c>
+      <c r="BL49" s="2">
+        <v>681</v>
+      </c>
     </row>
-    <row r="50" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
@@ -10844,8 +10991,11 @@
       <c r="BK50" s="2">
         <v>92</v>
       </c>
+      <c r="BL50" s="2">
+        <v>93</v>
+      </c>
     </row>
-    <row r="51" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
@@ -11035,8 +11185,11 @@
       <c r="BK51" s="2">
         <v>1598</v>
       </c>
+      <c r="BL51" s="2">
+        <v>1607</v>
+      </c>
     </row>
-    <row r="52" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>50</v>
       </c>
@@ -11226,8 +11379,11 @@
       <c r="BK52" s="2">
         <v>5331</v>
       </c>
+      <c r="BL52" s="2">
+        <v>6734</v>
+      </c>
     </row>
-    <row r="53" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
@@ -11417,8 +11573,11 @@
       <c r="BK53" s="2">
         <v>37</v>
       </c>
+      <c r="BL53" s="2">
+        <v>37</v>
+      </c>
     </row>
-    <row r="54" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>52</v>
       </c>
@@ -11608,8 +11767,11 @@
       <c r="BK54" s="2">
         <v>156</v>
       </c>
+      <c r="BL54" s="2">
+        <v>157</v>
+      </c>
     </row>
-    <row r="55" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -11799,8 +11961,11 @@
       <c r="BK55" s="2">
         <v>108</v>
       </c>
+      <c r="BL55" s="2">
+        <v>109</v>
+      </c>
     </row>
-    <row r="56" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>54</v>
       </c>
@@ -11990,8 +12155,11 @@
       <c r="BK56" s="2">
         <v>159</v>
       </c>
+      <c r="BL56" s="2">
+        <v>159</v>
+      </c>
     </row>
-    <row r="57" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>55</v>
       </c>
@@ -12181,8 +12349,11 @@
       <c r="BK57" s="2">
         <v>35</v>
       </c>
+      <c r="BL57" s="2">
+        <v>38</v>
+      </c>
     </row>
-    <row r="58" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>56</v>
       </c>
@@ -12372,8 +12543,11 @@
       <c r="BK58" s="2">
         <v>10</v>
       </c>
+      <c r="BL58" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="59" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>57</v>
       </c>
@@ -12563,8 +12737,11 @@
       <c r="BK59" s="2">
         <v>148824</v>
       </c>
+      <c r="BL59" s="2">
+        <v>152018</v>
+      </c>
     </row>
-    <row r="60" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
@@ -12754,8 +12931,11 @@
       <c r="BK60" s="2">
         <v>404</v>
       </c>
+      <c r="BL60" s="2">
+        <v>444</v>
+      </c>
     </row>
-    <row r="61" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>59</v>
       </c>
@@ -12945,8 +13125,11 @@
       <c r="BK61" s="2">
         <v>419</v>
       </c>
+      <c r="BL61" s="2">
+        <v>424</v>
+      </c>
     </row>
-    <row r="62" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>60</v>
       </c>
@@ -13136,8 +13319,11 @@
       <c r="BK62" s="2">
         <v>99</v>
       </c>
+      <c r="BL62" s="2">
+        <v>101</v>
+      </c>
     </row>
-    <row r="63" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>61</v>
       </c>
@@ -13327,8 +13513,11 @@
       <c r="BK63" s="2">
         <v>34901</v>
       </c>
+      <c r="BL63" s="2">
+        <v>35563</v>
+      </c>
     </row>
-    <row r="64" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>62</v>
       </c>
@@ -13518,8 +13707,11 @@
       <c r="BK64" s="2">
         <v>516</v>
       </c>
+      <c r="BL64" s="2">
+        <v>520</v>
+      </c>
     </row>
-    <row r="65" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>63</v>
       </c>
@@ -13709,8 +13901,11 @@
       <c r="BK65" s="2">
         <v>26</v>
       </c>
+      <c r="BL65" s="2">
+        <v>26</v>
+      </c>
     </row>
-    <row r="66" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>64</v>
       </c>
@@ -13900,8 +14095,11 @@
       <c r="BK66" s="2">
         <v>187</v>
       </c>
+      <c r="BL66" s="2">
+        <v>187</v>
+      </c>
     </row>
-    <row r="67" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>65</v>
       </c>
@@ -14091,8 +14289,11 @@
       <c r="BK67" s="2">
         <v>188</v>
       </c>
+      <c r="BL67" s="2">
+        <v>190</v>
+      </c>
     </row>
-    <row r="68" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>66</v>
       </c>
@@ -14282,8 +14483,11 @@
       <c r="BK68" s="2">
         <v>381</v>
       </c>
+      <c r="BL68" s="2">
+        <v>386</v>
+      </c>
     </row>
-    <row r="69" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>67</v>
       </c>
@@ -14473,8 +14677,11 @@
       <c r="BK69" s="2">
         <v>406</v>
       </c>
+      <c r="BL69" s="2">
+        <v>419</v>
+      </c>
     </row>
-    <row r="70" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>68</v>
       </c>
@@ -14664,8 +14871,11 @@
       <c r="BK70" s="2">
         <v>4696</v>
       </c>
+      <c r="BL70" s="2">
+        <v>4712</v>
+      </c>
     </row>
-    <row r="71" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>69</v>
       </c>
@@ -14855,8 +15065,11 @@
       <c r="BK71" s="2">
         <v>31</v>
       </c>
+      <c r="BL71" s="2">
+        <v>31</v>
+      </c>
     </row>
-    <row r="72" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>70</v>
       </c>
@@ -15046,8 +15259,11 @@
       <c r="BK72" s="2">
         <v>8877</v>
       </c>
+      <c r="BL72" s="2">
+        <v>9005</v>
+      </c>
     </row>
-    <row r="73" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>71</v>
       </c>
@@ -15237,8 +15453,11 @@
       <c r="BK73" s="2">
         <v>43758</v>
       </c>
+      <c r="BL73" s="2">
+        <v>44256</v>
+      </c>
     </row>
-    <row r="74" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>72</v>
       </c>
@@ -15428,8 +15647,11 @@
       <c r="BK74" s="2">
         <v>1490</v>
       </c>
+      <c r="BL74" s="2">
+        <v>1516</v>
+      </c>
     </row>
-    <row r="75" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>73</v>
       </c>
@@ -15619,8 +15841,11 @@
       <c r="BK75" s="2">
         <v>829</v>
       </c>
+      <c r="BL75" s="2">
+        <v>847</v>
+      </c>
     </row>
-    <row r="76" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>74</v>
       </c>
@@ -15810,8 +16035,11 @@
       <c r="BK76" s="2">
         <v>1406</v>
       </c>
+      <c r="BL76" s="2">
+        <v>1432</v>
+      </c>
     </row>
-    <row r="77" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>75</v>
       </c>
@@ -16001,8 +16229,11 @@
       <c r="BK77" s="2">
         <v>1373</v>
       </c>
+      <c r="BL77" s="2">
+        <v>1466</v>
+      </c>
     </row>
-    <row r="78" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>76</v>
       </c>
@@ -16192,8 +16423,11 @@
       <c r="BK78" s="2">
         <v>32</v>
       </c>
+      <c r="BL78" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="79" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>77</v>
       </c>
@@ -16383,8 +16617,11 @@
       <c r="BK79" s="2">
         <v>278</v>
       </c>
+      <c r="BL79" s="2">
+        <v>279</v>
+      </c>
     </row>
-    <row r="80" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>78</v>
       </c>
@@ -16574,8 +16811,11 @@
       <c r="BK80" s="2">
         <v>96</v>
       </c>
+      <c r="BL80" s="2">
+        <v>96</v>
+      </c>
     </row>
-    <row r="81" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>79</v>
       </c>
@@ -16765,8 +17005,11 @@
       <c r="BK81" s="2">
         <v>87927</v>
       </c>
+      <c r="BL81" s="2">
+        <v>89616</v>
+      </c>
     </row>
-    <row r="82" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>80</v>
       </c>
@@ -16956,8 +17199,11 @@
       <c r="BK82" s="2">
         <v>256</v>
       </c>
+      <c r="BL82" s="2">
+        <v>262</v>
+      </c>
     </row>
-    <row r="83" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>81</v>
       </c>
@@ -17147,8 +17393,11 @@
       <c r="BK83" s="2">
         <v>654</v>
       </c>
+      <c r="BL83" s="2">
+        <v>680</v>
+      </c>
     </row>
-    <row r="84" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>82</v>
       </c>
@@ -17338,8 +17587,11 @@
       <c r="BK84" s="2">
         <v>744</v>
       </c>
+      <c r="BL84" s="2">
+        <v>748</v>
+      </c>
     </row>
-    <row r="85" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>83</v>
       </c>
@@ -17529,8 +17781,11 @@
       <c r="BK85" s="2">
         <v>263</v>
       </c>
+      <c r="BL85" s="2">
+        <v>275</v>
+      </c>
     </row>
-    <row r="86" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>84</v>
       </c>
@@ -17720,8 +17975,11 @@
       <c r="BK86" s="2">
         <v>37765</v>
       </c>
+      <c r="BL86" s="2">
+        <v>38251</v>
+      </c>
     </row>
-    <row r="87" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -17911,8 +18169,11 @@
       <c r="BK87" s="2">
         <v>3</v>
       </c>
+      <c r="BL87" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="88" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>86</v>
       </c>
@@ -18102,8 +18363,11 @@
       <c r="BK88" s="2">
         <v>1006</v>
       </c>
+      <c r="BL88" s="2">
+        <v>1005</v>
+      </c>
     </row>
-    <row r="89" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>87</v>
       </c>
@@ -18293,8 +18557,11 @@
       <c r="BK89" s="2">
         <v>72</v>
       </c>
+      <c r="BL89" s="2">
+        <v>72</v>
+      </c>
     </row>
-    <row r="90" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>88</v>
       </c>
@@ -18484,8 +18751,11 @@
       <c r="BK90" s="2">
         <v>170</v>
       </c>
+      <c r="BL90" s="2">
+        <v>177</v>
+      </c>
     </row>
-    <row r="91" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>89</v>
       </c>
@@ -18675,8 +18945,11 @@
       <c r="BK91" s="2">
         <v>1082</v>
       </c>
+      <c r="BL91" s="2">
+        <v>1091</v>
+      </c>
     </row>
-    <row r="92" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>90</v>
       </c>
@@ -18866,8 +19139,11 @@
       <c r="BK92" s="2">
         <v>837</v>
       </c>
+      <c r="BL92" s="2">
+        <v>862</v>
+      </c>
     </row>
-    <row r="93" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>91</v>
       </c>
@@ -19057,8 +19333,11 @@
       <c r="BK93" s="2">
         <v>7306</v>
       </c>
+      <c r="BL93" s="2">
+        <v>7378</v>
+      </c>
     </row>
-    <row r="94" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>92</v>
       </c>
@@ -19248,8 +19527,11 @@
       <c r="BK94" s="2">
         <v>3014</v>
       </c>
+      <c r="BL94" s="2">
+        <v>3027</v>
+      </c>
     </row>
-    <row r="95" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>93</v>
       </c>
@@ -19439,8 +19721,11 @@
       <c r="BK95" s="2">
         <v>1071</v>
       </c>
+      <c r="BL95" s="2">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="96" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>94</v>
       </c>
@@ -19630,8 +19915,11 @@
       <c r="BK96" s="2">
         <v>3605</v>
       </c>
+      <c r="BL96" s="2">
+        <v>3736</v>
+      </c>
     </row>
-    <row r="97" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>95</v>
       </c>
@@ -19821,8 +20109,11 @@
       <c r="BK97" s="2">
         <v>427</v>
       </c>
+      <c r="BL97" s="2">
+        <v>436</v>
+      </c>
     </row>
-    <row r="98" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>96</v>
       </c>
@@ -20012,8 +20303,11 @@
       <c r="BK98" s="2">
         <v>161</v>
       </c>
+      <c r="BL98" s="2">
+        <v>161</v>
+      </c>
     </row>
-    <row r="99" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>97</v>
       </c>
@@ -20203,8 +20497,11 @@
       <c r="BK99" s="2">
         <v>776</v>
       </c>
+      <c r="BL99" s="2">
+        <v>784</v>
+      </c>
     </row>
-    <row r="100" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>98</v>
       </c>
@@ -20394,8 +20691,11 @@
       <c r="BK100" s="2">
         <v>54</v>
       </c>
+      <c r="BL100" s="2">
+        <v>55</v>
+      </c>
     </row>
-    <row r="101" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>99</v>
       </c>
@@ -20585,8 +20885,11 @@
       <c r="BK101" s="2">
         <v>59</v>
       </c>
+      <c r="BL101" s="2">
+        <v>60</v>
+      </c>
     </row>
-    <row r="102" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>100</v>
       </c>
@@ -20776,8 +21079,11 @@
       <c r="BK102" s="2">
         <v>879</v>
       </c>
+      <c r="BL102" s="2">
+        <v>903</v>
+      </c>
     </row>
-    <row r="103" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>101</v>
       </c>
@@ -20967,8 +21273,11 @@
       <c r="BK103" s="2">
         <v>252994</v>
       </c>
+      <c r="BL103" s="2">
+        <v>257823</v>
+      </c>
     </row>
-    <row r="104" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>102</v>
       </c>
@@ -21158,8 +21467,11 @@
       <c r="BK104" s="2">
         <v>4589</v>
       </c>
+      <c r="BL104" s="2">
+        <v>4654</v>
+      </c>
     </row>
-    <row r="105" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>103</v>
       </c>
@@ -21349,8 +21661,11 @@
       <c r="BK105" s="2">
         <v>87</v>
       </c>
+      <c r="BL105" s="2">
+        <v>89</v>
+      </c>
     </row>
-    <row r="106" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>104</v>
       </c>
@@ -21540,8 +21855,11 @@
       <c r="BK106" s="2">
         <v>284</v>
       </c>
+      <c r="BL106" s="2">
+        <v>286</v>
+      </c>
     </row>
-    <row r="107" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>105</v>
       </c>
@@ -21731,8 +22049,11 @@
       <c r="BK107" s="2">
         <v>10559</v>
       </c>
+      <c r="BL107" s="2">
+        <v>10923</v>
+      </c>
     </row>
-    <row r="108" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>106</v>
       </c>
@@ -21922,8 +22243,11 @@
       <c r="BK108" s="2">
         <v>179</v>
       </c>
+      <c r="BL108" s="2">
+        <v>182</v>
+      </c>
     </row>
-    <row r="109" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>107</v>
       </c>
@@ -22113,8 +22437,11 @@
       <c r="BK109" s="2">
         <v>1903</v>
       </c>
+      <c r="BL109" s="2">
+        <v>1959</v>
+      </c>
     </row>
-    <row r="110" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>108</v>
       </c>
@@ -22304,8 +22631,11 @@
       <c r="BK110" s="2">
         <v>23149</v>
       </c>
+      <c r="BL110" s="2">
+        <v>23699</v>
+      </c>
     </row>
-    <row r="111" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>109</v>
       </c>
@@ -22495,8 +22825,11 @@
       <c r="BK111" s="2">
         <v>1255</v>
       </c>
+      <c r="BL111" s="2">
+        <v>1267</v>
+      </c>
     </row>
-    <row r="112" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>110</v>
       </c>
@@ -22686,8 +23019,11 @@
       <c r="BK112" s="2">
         <v>93</v>
       </c>
+      <c r="BL112" s="2">
+        <v>94</v>
+      </c>
     </row>
-    <row r="113" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>111</v>
       </c>
@@ -22877,8 +23213,11 @@
       <c r="BK113" s="2">
         <v>1209</v>
       </c>
+      <c r="BL113" s="2">
+        <v>1227</v>
+      </c>
     </row>
-    <row r="114" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>112</v>
       </c>
@@ -23068,8 +23407,11 @@
       <c r="BK114" s="2">
         <v>690</v>
       </c>
+      <c r="BL114" s="2">
+        <v>721</v>
+      </c>
     </row>
-    <row r="115" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>113</v>
       </c>
@@ -23259,8 +23601,11 @@
       <c r="BK115" s="2">
         <v>799</v>
       </c>
+      <c r="BL115" s="2">
+        <v>1588</v>
+      </c>
     </row>
-    <row r="116" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>114</v>
       </c>
@@ -23450,8 +23795,11 @@
       <c r="BK116" s="2">
         <v>382</v>
       </c>
+      <c r="BL116" s="2">
+        <v>399</v>
+      </c>
     </row>
-    <row r="117" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>115</v>
       </c>
@@ -23641,8 +23989,11 @@
       <c r="BK117" s="2">
         <v>57</v>
       </c>
+      <c r="BL117" s="2">
+        <v>58</v>
+      </c>
     </row>
-    <row r="118" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>116</v>
       </c>
@@ -23832,8 +24183,11 @@
       <c r="BK118" s="2">
         <v>3859</v>
       </c>
+      <c r="BL118" s="2">
+        <v>3903</v>
+      </c>
     </row>
-    <row r="119" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>117</v>
       </c>
@@ -24023,8 +24377,11 @@
       <c r="BK119" s="2">
         <v>610</v>
       </c>
+      <c r="BL119" s="2">
+        <v>637</v>
+      </c>
     </row>
-    <row r="120" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>118</v>
       </c>
@@ -24214,8 +24571,11 @@
       <c r="BK120" s="2">
         <v>6</v>
       </c>
+      <c r="BL120" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="121" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>119</v>
       </c>
@@ -24405,8 +24765,11 @@
       <c r="BK121" s="2">
         <v>106</v>
       </c>
+      <c r="BL121" s="2">
+        <v>106</v>
+      </c>
     </row>
-    <row r="122" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>120</v>
       </c>
@@ -24596,8 +24959,11 @@
       <c r="BK122" s="2">
         <v>884</v>
       </c>
+      <c r="BL122" s="2">
+        <v>884</v>
+      </c>
     </row>
-    <row r="123" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>121</v>
       </c>
@@ -24787,8 +25153,11 @@
       <c r="BK123" s="2">
         <v>847</v>
       </c>
+      <c r="BL123" s="2">
+        <v>869</v>
+      </c>
     </row>
-    <row r="124" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>122</v>
       </c>
@@ -24978,8 +25347,11 @@
       <c r="BK124" s="2">
         <v>11</v>
       </c>
+      <c r="BL124" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="125" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>123</v>
       </c>
@@ -25169,8 +25541,11 @@
       <c r="BK125" s="2">
         <v>13662</v>
       </c>
+      <c r="BL125" s="2">
+        <v>15052</v>
+      </c>
     </row>
-    <row r="126" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>124</v>
       </c>
@@ -25360,8 +25735,11 @@
       <c r="BK126" s="2">
         <v>131</v>
       </c>
+      <c r="BL126" s="2">
+        <v>132</v>
+      </c>
     </row>
-    <row r="127" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>125</v>
       </c>
@@ -25551,8 +25929,11 @@
       <c r="BK127" s="2">
         <v>2142</v>
       </c>
+      <c r="BL127" s="2">
+        <v>2211</v>
+      </c>
     </row>
-    <row r="128" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
         <v>126</v>
       </c>
@@ -25742,8 +26123,11 @@
       <c r="BK128" s="2">
         <v>7874</v>
       </c>
+      <c r="BL128" s="2">
+        <v>8010</v>
+      </c>
     </row>
-    <row r="129" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>127</v>
       </c>
@@ -25933,8 +26317,11 @@
       <c r="BK129" s="2">
         <v>577</v>
       </c>
+      <c r="BL129" s="2">
+        <v>605</v>
+      </c>
     </row>
-    <row r="130" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
         <v>128</v>
       </c>
@@ -26124,8 +26511,11 @@
       <c r="BK130" s="2">
         <v>301</v>
       </c>
+      <c r="BL130" s="2">
+        <v>322</v>
+      </c>
     </row>
-    <row r="131" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>129</v>
       </c>
@@ -26315,8 +26705,11 @@
       <c r="BK131" s="2">
         <v>4544</v>
       </c>
+      <c r="BL131" s="2">
+        <v>4649</v>
+      </c>
     </row>
-    <row r="132" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
         <v>130</v>
       </c>
@@ -26506,8 +26899,11 @@
       <c r="BK132" s="2">
         <v>1275</v>
       </c>
+      <c r="BL132" s="2">
+        <v>1296</v>
+      </c>
     </row>
-    <row r="133" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>131</v>
       </c>
@@ -26697,8 +27093,11 @@
       <c r="BK133" s="2">
         <v>3</v>
       </c>
+      <c r="BL133" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="134" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>132</v>
       </c>
@@ -26888,8 +27287,11 @@
       <c r="BK134" s="2">
         <v>3</v>
       </c>
+      <c r="BL134" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="135" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>133</v>
       </c>
@@ -27079,8 +27481,11 @@
       <c r="BK135" s="2">
         <v>2290</v>
       </c>
+      <c r="BL135" s="2">
+        <v>2293</v>
+      </c>
     </row>
-    <row r="136" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
         <v>134</v>
       </c>
@@ -27270,8 +27675,11 @@
       <c r="BK136" s="2">
         <v>125</v>
       </c>
+      <c r="BL136" s="2">
+        <v>130</v>
+      </c>
     </row>
-    <row r="137" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>135</v>
       </c>
@@ -27461,8 +27869,11 @@
       <c r="BK137" s="2">
         <v>4</v>
       </c>
+      <c r="BL137" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="138" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
         <v>136</v>
       </c>
@@ -27652,8 +28063,11 @@
       <c r="BK138" s="2">
         <v>23</v>
       </c>
+      <c r="BL138" s="2">
+        <v>23</v>
+      </c>
     </row>
-    <row r="139" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>137</v>
       </c>
@@ -27843,8 +28257,11 @@
       <c r="BK139" s="2">
         <v>2276</v>
       </c>
+      <c r="BL139" s="2">
+        <v>2343</v>
+      </c>
     </row>
-    <row r="140" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>138</v>
       </c>
@@ -28034,8 +28451,11 @@
       <c r="BK140" s="2">
         <v>209</v>
       </c>
+      <c r="BL140" s="2">
+        <v>210</v>
+      </c>
     </row>
-    <row r="141" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>139</v>
       </c>
@@ -28225,8 +28645,11 @@
       <c r="BK141" s="2">
         <v>1348</v>
       </c>
+      <c r="BL141" s="2">
+        <v>1361</v>
+      </c>
     </row>
-    <row r="142" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
         <v>140</v>
       </c>
@@ -28416,8 +28839,11 @@
       <c r="BK142" s="2">
         <v>215</v>
       </c>
+      <c r="BL142" s="2">
+        <v>216</v>
+      </c>
     </row>
-    <row r="143" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
         <v>141</v>
       </c>
@@ -28607,8 +29033,11 @@
       <c r="BK143" s="2">
         <v>1506</v>
       </c>
+      <c r="BL143" s="2">
+        <v>1536</v>
+      </c>
     </row>
-    <row r="144" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
         <v>142</v>
       </c>
@@ -28798,8 +29227,11 @@
       <c r="BK144" s="2">
         <v>525</v>
       </c>
+      <c r="BL144" s="2">
+        <v>529</v>
+      </c>
     </row>
-    <row r="145" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
         <v>143</v>
       </c>
@@ -28989,8 +29421,11 @@
       <c r="BK145" s="2">
         <v>664</v>
       </c>
+      <c r="BL145" s="2">
+        <v>677</v>
+      </c>
     </row>
-    <row r="146" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
         <v>144</v>
       </c>
@@ -29180,8 +29615,11 @@
       <c r="BK146" s="2">
         <v>365</v>
       </c>
+      <c r="BL146" s="2">
+        <v>369</v>
+      </c>
     </row>
-    <row r="147" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
         <v>145</v>
       </c>
@@ -29371,8 +29809,11 @@
       <c r="BK147" s="2">
         <v>544</v>
       </c>
+      <c r="BL147" s="2">
+        <v>569</v>
+      </c>
     </row>
-    <row r="148" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>146</v>
       </c>
@@ -29562,8 +30003,11 @@
       <c r="BK148" s="2">
         <v>3374</v>
       </c>
+      <c r="BL148" s="2">
+        <v>3438</v>
+      </c>
     </row>
-    <row r="149" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>147</v>
       </c>
@@ -29753,8 +30197,11 @@
       <c r="BK149" s="2">
         <v>904</v>
       </c>
+      <c r="BL149" s="2">
+        <v>923</v>
+      </c>
     </row>
-    <row r="150" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>148</v>
       </c>
@@ -29944,8 +30391,11 @@
       <c r="BK150" s="2">
         <v>120</v>
       </c>
+      <c r="BL150" s="2">
+        <v>120</v>
+      </c>
     </row>
-    <row r="151" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
         <v>149</v>
       </c>
@@ -30135,8 +30585,11 @@
       <c r="BK151" s="2">
         <v>390</v>
       </c>
+      <c r="BL151" s="2">
+        <v>391</v>
+      </c>
     </row>
-    <row r="152" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>150</v>
       </c>
@@ -30326,8 +30779,11 @@
       <c r="BK152" s="2">
         <v>1137</v>
       </c>
+      <c r="BL152" s="2">
+        <v>1149</v>
+      </c>
     </row>
-    <row r="153" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
         <v>151</v>
       </c>
@@ -30517,8 +30973,11 @@
       <c r="BK153" s="2">
         <v>1</v>
       </c>
+      <c r="BL153" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="154" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>152</v>
       </c>
@@ -30708,8 +31167,11 @@
       <c r="BK154" s="2">
         <v>12984</v>
       </c>
+      <c r="BL154" s="2">
+        <v>13101</v>
+      </c>
     </row>
-    <row r="155" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
         <v>153</v>
       </c>
@@ -30899,8 +31361,11 @@
       <c r="BK155" s="2">
         <v>463</v>
       </c>
+      <c r="BL155" s="2">
+        <v>475</v>
+      </c>
     </row>
-    <row r="156" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>154</v>
       </c>
@@ -31090,8 +31555,11 @@
       <c r="BK156" s="2">
         <v>94</v>
       </c>
+      <c r="BL156" s="2">
+        <v>92</v>
+      </c>
     </row>
-    <row r="157" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
         <v>155</v>
       </c>
@@ -31281,8 +31749,11 @@
       <c r="BK157" s="2">
         <v>13300</v>
       </c>
+      <c r="BL157" s="2">
+        <v>13407</v>
+      </c>
     </row>
-    <row r="158" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>156</v>
       </c>
@@ -31472,8 +31943,11 @@
       <c r="BK158" s="2">
         <v>11</v>
       </c>
+      <c r="BL158" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="159" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
         <v>157</v>
       </c>
@@ -31663,8 +32137,11 @@
       <c r="BK159" s="2">
         <v>538</v>
       </c>
+      <c r="BL159" s="2">
+        <v>582</v>
+      </c>
     </row>
-    <row r="160" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>158</v>
       </c>
@@ -31854,8 +32331,11 @@
       <c r="BK160" s="2">
         <v>103</v>
       </c>
+      <c r="BL160" s="2">
+        <v>105</v>
+      </c>
     </row>
-    <row r="161" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
         <v>159</v>
       </c>
@@ -32045,8 +32525,11 @@
       <c r="BK161" s="2">
         <v>109</v>
       </c>
+      <c r="BL161" s="2">
+        <v>110</v>
+      </c>
     </row>
-    <row r="162" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>160</v>
       </c>
@@ -32236,8 +32719,11 @@
       <c r="BK162" s="2">
         <v>354</v>
       </c>
+      <c r="BL162" s="2">
+        <v>353</v>
+      </c>
     </row>
-    <row r="163" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
         <v>161</v>
       </c>
@@ -32427,8 +32913,11 @@
       <c r="BK163" s="2">
         <v>1656</v>
       </c>
+      <c r="BL163" s="2">
+        <v>1667</v>
+      </c>
     </row>
-    <row r="164" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
         <v>162</v>
       </c>
@@ -32618,8 +33107,11 @@
       <c r="BK164" s="2">
         <v>3367</v>
       </c>
+      <c r="BL164" s="2">
+        <v>3408</v>
+      </c>
     </row>
-    <row r="165" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
         <v>163</v>
       </c>
@@ -32809,8 +33301,11 @@
       <c r="BK165" s="2">
         <v>1084</v>
       </c>
+      <c r="BL165" s="2">
+        <v>1135</v>
+      </c>
     </row>
-    <row r="166" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
         <v>164</v>
       </c>
@@ -33000,8 +33495,11 @@
       <c r="BK166" s="2">
         <v>31</v>
       </c>
+      <c r="BL166" s="2">
+        <v>31</v>
+      </c>
     </row>
-    <row r="167" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
         <v>165</v>
       </c>
@@ -33191,8 +33689,11 @@
       <c r="BK167" s="2">
         <v>5195</v>
       </c>
+      <c r="BL167" s="2">
+        <v>5273</v>
+      </c>
     </row>
-    <row r="168" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
         <v>166</v>
       </c>
@@ -33382,8 +33883,11 @@
       <c r="BK168" s="2">
         <v>1618</v>
       </c>
+      <c r="BL168" s="2">
+        <v>1630</v>
+      </c>
     </row>
-    <row r="169" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
         <v>167</v>
       </c>
@@ -33573,8 +34077,11 @@
       <c r="BK169" s="2">
         <v>108</v>
       </c>
+      <c r="BL169" s="2">
+        <v>108</v>
+      </c>
     </row>
-    <row r="170" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
         <v>168</v>
       </c>
@@ -33764,8 +34271,11 @@
       <c r="BK170" s="2">
         <v>214</v>
       </c>
+      <c r="BL170" s="2">
+        <v>226</v>
+      </c>
     </row>
-    <row r="171" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
         <v>169</v>
       </c>
@@ -33955,8 +34465,11 @@
       <c r="BK171" s="2">
         <v>323</v>
       </c>
+      <c r="BL171" s="2">
+        <v>326</v>
+      </c>
     </row>
-    <row r="172" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
         <v>170</v>
       </c>
@@ -34146,8 +34659,11 @@
       <c r="BK172" s="2">
         <v>25762</v>
       </c>
+      <c r="BL172" s="2">
+        <v>26283</v>
+      </c>
     </row>
-    <row r="173" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>171</v>
       </c>
@@ -34337,8 +34853,11 @@
       <c r="BK173" s="2">
         <v>2900</v>
       </c>
+      <c r="BL173" s="2">
+        <v>2904</v>
+      </c>
     </row>
-    <row r="174" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
         <v>172</v>
       </c>
@@ -34528,8 +35047,11 @@
       <c r="BK174" s="2">
         <v>226</v>
       </c>
+      <c r="BL174" s="2">
+        <v>238</v>
+      </c>
     </row>
-    <row r="175" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
         <v>173</v>
       </c>
@@ -34719,8 +35241,11 @@
       <c r="BK175" s="2">
         <v>27</v>
       </c>
+      <c r="BL175" s="2">
+        <v>27</v>
+      </c>
     </row>
-    <row r="176" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
         <v>174</v>
       </c>
@@ -34910,8 +35435,11 @@
       <c r="BK176" s="2">
         <v>2941</v>
       </c>
+      <c r="BL176" s="2">
+        <v>2954</v>
+      </c>
     </row>
-    <row r="177" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
         <v>175</v>
       </c>
@@ -35101,8 +35629,11 @@
       <c r="BK177" s="2">
         <v>1663</v>
       </c>
+      <c r="BL177" s="2">
+        <v>1684</v>
+      </c>
     </row>
-    <row r="178" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
         <v>176</v>
       </c>
@@ -35292,8 +35823,11 @@
       <c r="BK178" s="2">
         <v>307</v>
       </c>
+      <c r="BL178" s="2">
+        <v>315</v>
+      </c>
     </row>
-    <row r="179" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>177</v>
       </c>
@@ -35483,8 +36017,11 @@
       <c r="BK179" s="2">
         <v>155</v>
       </c>
+      <c r="BL179" s="2">
+        <v>161</v>
+      </c>
     </row>
-    <row r="180" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
         <v>178</v>
       </c>
@@ -35674,8 +36211,11 @@
       <c r="BK180" s="2">
         <v>6255</v>
       </c>
+      <c r="BL180" s="2">
+        <v>6378</v>
+      </c>
     </row>
-    <row r="181" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>179</v>
       </c>
@@ -35865,8 +36405,11 @@
       <c r="BK181" s="2">
         <v>145</v>
       </c>
+      <c r="BL181" s="2">
+        <v>145</v>
+      </c>
     </row>
-    <row r="182" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
         <v>180</v>
       </c>
@@ -36056,8 +36599,11 @@
       <c r="BK182" s="2">
         <v>113</v>
       </c>
+      <c r="BL182" s="2">
+        <v>113</v>
+      </c>
     </row>
-    <row r="183" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>181</v>
       </c>
@@ -36247,8 +36793,11 @@
       <c r="BK183" s="2">
         <v>1492</v>
       </c>
+      <c r="BL183" s="2">
+        <v>1545</v>
+      </c>
     </row>
-    <row r="184" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>182</v>
       </c>
@@ -36438,8 +36987,11 @@
       <c r="BK184" s="2">
         <v>664</v>
       </c>
+      <c r="BL184" s="2">
+        <v>674</v>
+      </c>
     </row>
-    <row r="185" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>183</v>
       </c>
@@ -36629,8 +37181,11 @@
       <c r="BK185" s="2">
         <v>639</v>
       </c>
+      <c r="BL185" s="2">
+        <v>643</v>
+      </c>
     </row>
-    <row r="186" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
         <v>184</v>
       </c>
@@ -36820,8 +37375,11 @@
       <c r="BK186" s="2">
         <v>5303</v>
       </c>
+      <c r="BL186" s="2">
+        <v>5367</v>
+      </c>
     </row>
-    <row r="187" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>185</v>
       </c>
@@ -37011,8 +37569,11 @@
       <c r="BK187" s="2">
         <v>324</v>
       </c>
+      <c r="BL187" s="2">
+        <v>326</v>
+      </c>
     </row>
-    <row r="188" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
         <v>186</v>
       </c>
@@ -37202,8 +37763,11 @@
       <c r="BK188" s="2">
         <v>804</v>
       </c>
+      <c r="BL188" s="2">
+        <v>1136</v>
+      </c>
     </row>
-    <row r="189" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>187</v>
       </c>
@@ -37393,8 +37957,11 @@
       <c r="BK189" s="2">
         <v>1838</v>
       </c>
+      <c r="BL189" s="2">
+        <v>1915</v>
+      </c>
     </row>
-    <row r="190" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>188</v>
       </c>
@@ -37584,8 +38151,11 @@
       <c r="BK190" s="2">
         <v>12930</v>
       </c>
+      <c r="BL190" s="2">
+        <v>14204</v>
+      </c>
     </row>
-    <row r="191" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
         <v>189</v>
       </c>
@@ -37775,8 +38345,11 @@
       <c r="BK191" s="2">
         <v>132</v>
       </c>
+      <c r="BL191" s="2">
+        <v>133</v>
+      </c>
     </row>
-    <row r="192" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
         <v>190</v>
       </c>
@@ -37966,8 +38539,11 @@
       <c r="BK192" s="2">
         <v>112</v>
       </c>
+      <c r="BL192" s="2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="193" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
         <v>191</v>
       </c>
@@ -38157,8 +38733,11 @@
       <c r="BK193" s="2">
         <v>4862</v>
       </c>
+      <c r="BL193" s="2">
+        <v>5019</v>
+      </c>
     </row>
-    <row r="194" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>192</v>
       </c>
@@ -38348,8 +38927,11 @@
       <c r="BK194" s="2">
         <v>115</v>
       </c>
+      <c r="BL194" s="2">
+        <v>115</v>
+      </c>
     </row>
-    <row r="195" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>193</v>
       </c>
@@ -38539,8 +39121,11 @@
       <c r="BK195" s="2">
         <v>139</v>
       </c>
+      <c r="BL195" s="2">
+        <v>139</v>
+      </c>
     </row>
-    <row r="196" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
         <v>194</v>
       </c>
@@ -38730,8 +39315,11 @@
       <c r="BK196" s="2">
         <v>403</v>
       </c>
+      <c r="BL196" s="2">
+        <v>418</v>
+      </c>
     </row>
-    <row r="197" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>195</v>
       </c>
@@ -38921,8 +39509,11 @@
       <c r="BK197" s="2">
         <v>235</v>
       </c>
+      <c r="BL197" s="2">
+        <v>235</v>
+      </c>
     </row>
-    <row r="198" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
         <v>196</v>
       </c>
@@ -39112,8 +39703,11 @@
       <c r="BK198" s="2">
         <v>208</v>
       </c>
+      <c r="BL198" s="2">
+        <v>213</v>
+      </c>
     </row>
-    <row r="199" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>197</v>
       </c>
@@ -39303,8 +39897,11 @@
       <c r="BK199" s="2">
         <v>7</v>
       </c>
+      <c r="BL199" s="2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="200" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>198</v>
       </c>
@@ -39494,8 +40091,11 @@
       <c r="BK200" s="2">
         <v>692</v>
       </c>
+      <c r="BL200" s="2">
+        <v>701</v>
+      </c>
     </row>
-    <row r="201" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
         <v>199</v>
       </c>
@@ -39685,8 +40285,11 @@
       <c r="BK201" s="2">
         <v>4813</v>
       </c>
+      <c r="BL201" s="2">
+        <v>4882</v>
+      </c>
     </row>
-    <row r="202" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>200</v>
       </c>
@@ -39876,8 +40479,11 @@
       <c r="BK202" s="2">
         <v>331</v>
       </c>
+      <c r="BL202" s="2">
+        <v>335</v>
+      </c>
     </row>
-    <row r="203" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
         <v>201</v>
       </c>
@@ -40067,8 +40673,11 @@
       <c r="BK203" s="2">
         <v>1280</v>
       </c>
+      <c r="BL203" s="2">
+        <v>1291</v>
+      </c>
     </row>
-    <row r="204" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>202</v>
       </c>
@@ -40258,8 +40867,11 @@
       <c r="BK204" s="2">
         <v>514</v>
       </c>
+      <c r="BL204" s="2">
+        <v>517</v>
+      </c>
     </row>
-    <row r="205" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A205" s="5" t="s">
         <v>203</v>
       </c>
@@ -40449,8 +41061,11 @@
       <c r="BK205" s="2">
         <v>296</v>
       </c>
+      <c r="BL205" s="2">
+        <v>298</v>
+      </c>
     </row>
-    <row r="206" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
         <v>204</v>
       </c>
@@ -40640,8 +41255,11 @@
       <c r="BK206" s="2">
         <v>646</v>
       </c>
+      <c r="BL206" s="2">
+        <v>691</v>
+      </c>
     </row>
-    <row r="207" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
         <v>205</v>
       </c>
@@ -40831,8 +41449,11 @@
       <c r="BK207" s="2">
         <v>1180</v>
       </c>
+      <c r="BL207" s="2">
+        <v>1210</v>
+      </c>
     </row>
-    <row r="208" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
         <v>206</v>
       </c>
@@ -41022,8 +41643,11 @@
       <c r="BK208" s="2">
         <v>197</v>
       </c>
+      <c r="BL208" s="2">
+        <v>197</v>
+      </c>
     </row>
-    <row r="209" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>207</v>
       </c>
@@ -41213,8 +41837,11 @@
       <c r="BK209" s="2">
         <v>102</v>
       </c>
+      <c r="BL209" s="2">
+        <v>106</v>
+      </c>
     </row>
-    <row r="210" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
         <v>208</v>
       </c>
@@ -41404,8 +42031,11 @@
       <c r="BK210" s="2">
         <v>99</v>
       </c>
+      <c r="BL210" s="2">
+        <v>103</v>
+      </c>
     </row>
-    <row r="211" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A211" s="5" t="s">
         <v>209</v>
       </c>
@@ -41595,8 +42225,11 @@
       <c r="BK211" s="2">
         <v>41</v>
       </c>
+      <c r="BL211" s="2">
+        <v>44</v>
+      </c>
     </row>
-    <row r="212" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A212" s="5" t="s">
         <v>210</v>
       </c>
@@ -41786,8 +42419,11 @@
       <c r="BK212" s="2">
         <v>1474</v>
       </c>
+      <c r="BL212" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="213" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A213" s="5" t="s">
         <v>211</v>
       </c>
@@ -41977,8 +42613,11 @@
       <c r="BK213" s="2">
         <v>35</v>
       </c>
+      <c r="BL213" s="2">
+        <v>35</v>
+      </c>
     </row>
-    <row r="214" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>212</v>
       </c>
@@ -42168,8 +42807,11 @@
       <c r="BK214" s="2">
         <v>7050</v>
       </c>
+      <c r="BL214" s="2">
+        <v>7212</v>
+      </c>
     </row>
-    <row r="215" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
         <v>213</v>
       </c>
@@ -42359,8 +43001,11 @@
       <c r="BK215" s="2">
         <v>290</v>
       </c>
+      <c r="BL215" s="2">
+        <v>290</v>
+      </c>
     </row>
-    <row r="216" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>214</v>
       </c>
@@ -42550,8 +43195,11 @@
       <c r="BK216" s="2">
         <v>2124</v>
       </c>
+      <c r="BL216" s="2">
+        <v>2639</v>
+      </c>
     </row>
-    <row r="217" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A217" s="5" t="s">
         <v>215</v>
       </c>
@@ -42741,8 +43389,11 @@
       <c r="BK217" s="2">
         <v>103</v>
       </c>
+      <c r="BL217" s="2">
+        <v>113</v>
+      </c>
     </row>
-    <row r="218" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A218" s="5" t="s">
         <v>216</v>
       </c>
@@ -42932,8 +43583,11 @@
       <c r="BK218" s="2">
         <v>26</v>
       </c>
+      <c r="BL218" s="2">
+        <v>27</v>
+      </c>
     </row>
-    <row r="219" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A219" s="5" t="s">
         <v>217</v>
       </c>
@@ -43123,8 +43777,11 @@
       <c r="BK219" s="2">
         <v>9</v>
       </c>
+      <c r="BL219" s="2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="220" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>218</v>
       </c>
@@ -43314,8 +43971,11 @@
       <c r="BK220" s="2">
         <v>60</v>
       </c>
+      <c r="BL220" s="2">
+        <v>64</v>
+      </c>
     </row>
-    <row r="221" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
         <v>219</v>
       </c>
@@ -43505,8 +44165,11 @@
       <c r="BK221" s="2">
         <v>236</v>
       </c>
+      <c r="BL221" s="2">
+        <v>254</v>
+      </c>
     </row>
-    <row r="222" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>220</v>
       </c>
@@ -43696,8 +44359,11 @@
       <c r="BK222" s="2">
         <v>87374</v>
       </c>
+      <c r="BL222" s="2">
+        <v>89133</v>
+      </c>
     </row>
-    <row r="223" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A223" s="5" t="s">
         <v>221</v>
       </c>
@@ -43887,8 +44553,11 @@
       <c r="BK223" s="2">
         <v>6740</v>
       </c>
+      <c r="BL223" s="2">
+        <v>8087</v>
+      </c>
     </row>
-    <row r="224" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
         <v>222</v>
       </c>
@@ -44078,8 +44747,11 @@
       <c r="BK224" s="2">
         <v>6</v>
       </c>
+      <c r="BL224" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="225" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A225" s="5" t="s">
         <v>223</v>
       </c>
@@ -44269,8 +44941,11 @@
       <c r="BK225" s="2">
         <v>262</v>
       </c>
+      <c r="BL225" s="2">
+        <v>271</v>
+      </c>
     </row>
-    <row r="226" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A226" s="5" t="s">
         <v>224</v>
       </c>
@@ -44460,8 +45135,11 @@
       <c r="BK226" s="2">
         <v>43</v>
       </c>
+      <c r="BL226" s="2">
+        <v>43</v>
+      </c>
     </row>
-    <row r="227" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A227" s="5" t="s">
         <v>225</v>
       </c>
@@ -44651,8 +45329,11 @@
       <c r="BK227" s="2">
         <v>2830</v>
       </c>
+      <c r="BL227" s="2">
+        <v>2850</v>
+      </c>
     </row>
-    <row r="228" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A228" s="5" t="s">
         <v>226</v>
       </c>
@@ -44842,8 +45523,11 @@
       <c r="BK228" s="2">
         <v>2667</v>
       </c>
+      <c r="BL228" s="2">
+        <v>2731</v>
+      </c>
     </row>
-    <row r="229" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A229" s="5" t="s">
         <v>227</v>
       </c>
@@ -45033,8 +45717,11 @@
       <c r="BK229" s="2">
         <v>54765</v>
       </c>
+      <c r="BL229" s="2">
+        <v>56384</v>
+      </c>
     </row>
-    <row r="230" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A230" s="5" t="s">
         <v>228</v>
       </c>
@@ -45224,8 +45911,11 @@
       <c r="BK230" s="2">
         <v>623</v>
       </c>
+      <c r="BL230" s="2">
+        <v>692</v>
+      </c>
     </row>
-    <row r="231" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A231" s="5" t="s">
         <v>229</v>
       </c>
@@ -45415,8 +46105,11 @@
       <c r="BK231" s="2">
         <v>624</v>
       </c>
+      <c r="BL231" s="2">
+        <v>662</v>
+      </c>
     </row>
-    <row r="232" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
         <v>230</v>
       </c>
@@ -45606,8 +46299,11 @@
       <c r="BK232" s="2">
         <v>442</v>
       </c>
+      <c r="BL232" s="2">
+        <v>447</v>
+      </c>
     </row>
-    <row r="233" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A233" s="5" t="s">
         <v>231</v>
       </c>
@@ -45797,8 +46493,11 @@
       <c r="BK233" s="2">
         <v>153</v>
       </c>
+      <c r="BL233" s="2">
+        <v>154</v>
+      </c>
     </row>
-    <row r="234" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A234" s="5" t="s">
         <v>232</v>
       </c>
@@ -45988,8 +46687,11 @@
       <c r="BK234" s="2">
         <v>884</v>
       </c>
+      <c r="BL234" s="2">
+        <v>895</v>
+      </c>
     </row>
-    <row r="235" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A235" s="5" t="s">
         <v>233</v>
       </c>
@@ -46179,8 +46881,11 @@
       <c r="BK235" s="2">
         <v>1413</v>
       </c>
+      <c r="BL235" s="2">
+        <v>1420</v>
+      </c>
     </row>
-    <row r="236" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A236" s="5" t="s">
         <v>234</v>
       </c>
@@ -46370,8 +47075,11 @@
       <c r="BK236" s="2">
         <v>1467</v>
       </c>
+      <c r="BL236" s="2">
+        <v>1484</v>
+      </c>
     </row>
-    <row r="237" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A237" s="5" t="s">
         <v>235</v>
       </c>
@@ -46561,8 +47269,11 @@
       <c r="BK237" s="2">
         <v>3648</v>
       </c>
+      <c r="BL237" s="2">
+        <v>3657</v>
+      </c>
     </row>
-    <row r="238" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A238" s="5" t="s">
         <v>236</v>
       </c>
@@ -46752,8 +47463,11 @@
       <c r="BK238" s="2">
         <v>8698</v>
       </c>
+      <c r="BL238" s="2">
+        <v>9659</v>
+      </c>
     </row>
-    <row r="239" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A239" s="5" t="s">
         <v>237</v>
       </c>
@@ -46943,8 +47657,11 @@
       <c r="BK239" s="2">
         <v>1751</v>
       </c>
+      <c r="BL239" s="2">
+        <v>1769</v>
+      </c>
     </row>
-    <row r="240" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A240" s="5" t="s">
         <v>238</v>
       </c>
@@ -47134,8 +47851,11 @@
       <c r="BK240" s="2">
         <v>245</v>
       </c>
+      <c r="BL240" s="2">
+        <v>249</v>
+      </c>
     </row>
-    <row r="241" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
         <v>239</v>
       </c>
@@ -47325,8 +48045,11 @@
       <c r="BK241" s="2">
         <v>2445</v>
       </c>
+      <c r="BL241" s="2">
+        <v>2484</v>
+      </c>
     </row>
-    <row r="242" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A242" s="5" t="s">
         <v>240</v>
       </c>
@@ -47516,8 +48239,11 @@
       <c r="BK242" s="2">
         <v>8181</v>
       </c>
+      <c r="BL242" s="2">
+        <v>8348</v>
+      </c>
     </row>
-    <row r="243" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A243" s="5" t="s">
         <v>241</v>
       </c>
@@ -47707,8 +48433,11 @@
       <c r="BK243" s="2">
         <v>2141</v>
       </c>
+      <c r="BL243" s="2">
+        <v>2187</v>
+      </c>
     </row>
-    <row r="244" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A244" s="5" t="s">
         <v>242</v>
       </c>
@@ -47898,8 +48627,11 @@
       <c r="BK244" s="2">
         <v>133</v>
       </c>
+      <c r="BL244" s="2">
+        <v>137</v>
+      </c>
     </row>
-    <row r="245" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A245" s="5" t="s">
         <v>243</v>
       </c>
@@ -48089,8 +48821,11 @@
       <c r="BK245" s="2">
         <v>6770</v>
       </c>
+      <c r="BL245" s="2">
+        <v>6876</v>
+      </c>
     </row>
-    <row r="246" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A246" s="5" t="s">
         <v>244</v>
       </c>
@@ -48280,8 +49015,11 @@
       <c r="BK246" s="2">
         <v>293</v>
       </c>
+      <c r="BL246" s="2">
+        <v>292</v>
+      </c>
     </row>
-    <row r="247" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A247" s="5" t="s">
         <v>245</v>
       </c>
@@ -48471,8 +49209,11 @@
       <c r="BK247" s="2">
         <v>1611</v>
       </c>
+      <c r="BL247" s="2">
+        <v>1635</v>
+      </c>
     </row>
-    <row r="248" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="s">
         <v>246</v>
       </c>
@@ -48662,8 +49403,11 @@
       <c r="BK248" s="2">
         <v>18762</v>
       </c>
+      <c r="BL248" s="2">
+        <v>19026</v>
+      </c>
     </row>
-    <row r="249" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A249" s="5" t="s">
         <v>247</v>
       </c>
@@ -48853,8 +49597,11 @@
       <c r="BK249" s="2">
         <v>1192</v>
       </c>
+      <c r="BL249" s="2">
+        <v>1213</v>
+      </c>
     </row>
-    <row r="250" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A250" s="5" t="s">
         <v>248</v>
       </c>
@@ -49044,8 +49791,11 @@
       <c r="BK250" s="2">
         <v>35</v>
       </c>
+      <c r="BL250" s="2">
+        <v>35</v>
+      </c>
     </row>
-    <row r="251" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A251" s="5" t="s">
         <v>249</v>
       </c>
@@ -49235,8 +49985,11 @@
       <c r="BK251" s="2">
         <v>1501</v>
       </c>
+      <c r="BL251" s="2">
+        <v>1516</v>
+      </c>
     </row>
-    <row r="252" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A252" s="5" t="s">
         <v>250</v>
       </c>
@@ -49426,8 +50179,11 @@
       <c r="BK252" s="2">
         <v>823</v>
       </c>
+      <c r="BL252" s="2">
+        <v>843</v>
+      </c>
     </row>
-    <row r="253" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A253" s="5" t="s">
         <v>251</v>
       </c>
@@ -49617,8 +50373,11 @@
       <c r="BK253" s="2">
         <v>220</v>
       </c>
+      <c r="BL253" s="2">
+        <v>221</v>
+      </c>
     </row>
-    <row r="254" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A254" s="5" t="s">
         <v>252</v>
       </c>
@@ -49808,8 +50567,11 @@
       <c r="BK254" s="2">
         <v>718</v>
       </c>
+      <c r="BL254" s="2">
+        <v>721</v>
+      </c>
     </row>
-    <row r="255" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A255" s="5" t="s">
         <v>253</v>
       </c>
@@ -49999,8 +50761,11 @@
       <c r="BK255" s="2">
         <v>440</v>
       </c>
+      <c r="BL255" s="2">
+        <v>523</v>
+      </c>
     </row>
-    <row r="256" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A256" s="5" t="s">
         <v>254</v>
       </c>
@@ -50190,8 +50955,11 @@
       <c r="BK256" s="2">
         <v>125</v>
       </c>
+      <c r="BL256" s="2">
+        <v>126</v>
+      </c>
     </row>
-    <row r="257" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A257" s="5" t="s">
         <v>255</v>
       </c>
@@ -50381,8 +51149,11 @@
       <c r="BK257" s="2">
         <v>4546</v>
       </c>
+      <c r="BL257" s="2">
+        <v>4580</v>
+      </c>
     </row>
-    <row r="258" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A258" s="5" t="s">
         <v>256</v>
       </c>
@@ -50573,8 +51344,11 @@
       <c r="BK258" s="2">
         <v>397366</v>
       </c>
+      <c r="BL258" s="2">
+        <v>412201</v>
+      </c>
     </row>
-    <row r="259" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A259" s="9" t="s">
         <v>257</v>
       </c>
@@ -50768,8 +51542,11 @@
       <c r="BK259" s="10">
         <v>1715177</v>
       </c>
+      <c r="BL259" s="10">
+        <v>1767701</v>
+      </c>
     </row>
-    <row r="261" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A261" s="3" t="s">
         <v>261</v>
       </c>
@@ -50782,7 +51559,7 @@
       <c r="H261" s="4"/>
       <c r="I261" s="4"/>
     </row>
-    <row r="262" spans="1:63" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" s="21" t="s">
         <v>258</v>
       </c>
@@ -50795,7 +51572,7 @@
       <c r="H262" s="22"/>
       <c r="I262" s="22"/>
     </row>
-    <row r="263" spans="1:63" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:64" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" s="23" t="s">
         <v>259</v>
       </c>
@@ -50808,7 +51585,7 @@
       <c r="H263" s="24"/>
       <c r="I263" s="24"/>
     </row>
-    <row r="264" spans="1:63" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:64" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" s="23" t="s">
         <v>260</v>
       </c>
@@ -50821,7 +51598,7 @@
       <c r="H264" s="24"/>
       <c r="I264" s="24"/>
     </row>
-    <row r="265" spans="1:63" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:64" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" s="11" t="s">
         <v>288</v>
       </c>
@@ -50884,9 +51661,9 @@
       <c r="BF265" s="13"/>
       <c r="BG265" s="13"/>
     </row>
-    <row r="266" spans="1:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B266" s="18"/>
       <c r="C266" s="13"/>
@@ -50897,7 +51674,7 @@
       <c r="H266" s="13"/>
       <c r="I266" s="13"/>
     </row>
-    <row r="267" spans="1:63" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:64" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" s="23" t="s">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
Update SF and TX for today 2020-06-26T04:24:05Z
</commit_message>
<xml_diff>
--- a/raw/TX/TexasCOVID-19CumulativeTestsOverTimebyCounty.xlsx
+++ b/raw/TX/TexasCOVID-19CumulativeTestsOverTimebyCounty.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1430C315-D6B2-439C-8E8F-4EB7CE9ECA2A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B07D47DE-09A7-488A-858B-A61906919571}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="332">
   <si>
     <t>County</t>
   </si>
@@ -1022,20 +1022,29 @@
     <t>Tests Through June 22</t>
   </si>
   <si>
-    <t>5. This file will be updated daily; the next cumulative update will be 6/24/2020.</t>
+    <t>Tests Through June 23</t>
+  </si>
+  <si>
+    <t>5. This file will be updated daily; the next cumulative update will be 6/26/2020.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1120,30 +1129,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1152,40 +1162,41 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1463,13 +1474,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL267"/>
+  <dimension ref="A1:BN267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A267" sqref="A267:I267"/>
+      <selection pane="bottomRight" activeCell="BM255" sqref="BM255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1480,16 +1491,15 @@
     <col min="40" max="45" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11.453125" style="2" customWidth="1"/>
     <col min="47" max="49" width="11.1796875" style="2" customWidth="1"/>
-    <col min="50" max="59" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="64" width="12.90625" customWidth="1"/>
+    <col min="50" max="66" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:66" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1682,8 +1692,14 @@
       <c r="BL2" s="7" t="s">
         <v>329</v>
       </c>
+      <c r="BM2" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>330</v>
+      </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1876,8 +1892,14 @@
       <c r="BL3" s="2">
         <v>5058</v>
       </c>
+      <c r="BM3" s="2">
+        <v>5730</v>
+      </c>
+      <c r="BN3" s="2">
+        <v>5803</v>
+      </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2070,8 +2092,14 @@
       <c r="BL4" s="2">
         <v>95</v>
       </c>
+      <c r="BM4" s="2">
+        <v>95</v>
+      </c>
+      <c r="BN4" s="2">
+        <v>95</v>
+      </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2264,8 +2292,14 @@
       <c r="BL5" s="2">
         <v>3662</v>
       </c>
+      <c r="BM5" s="2">
+        <v>3772</v>
+      </c>
+      <c r="BN5" s="2">
+        <v>3793</v>
+      </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2458,8 +2492,14 @@
       <c r="BL6" s="2">
         <v>342</v>
       </c>
+      <c r="BM6" s="2">
+        <v>356</v>
+      </c>
+      <c r="BN6" s="2">
+        <v>356</v>
+      </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2652,8 +2692,14 @@
       <c r="BL7" s="2">
         <v>94</v>
       </c>
+      <c r="BM7" s="2">
+        <v>98</v>
+      </c>
+      <c r="BN7" s="2">
+        <v>99</v>
+      </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2846,8 +2892,14 @@
       <c r="BL8" s="2">
         <v>180</v>
       </c>
+      <c r="BM8" s="2">
+        <v>180</v>
+      </c>
+      <c r="BN8" s="2">
+        <v>180</v>
+      </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -3040,8 +3092,14 @@
       <c r="BL9" s="2">
         <v>1424</v>
       </c>
+      <c r="BM9" s="2">
+        <v>1447</v>
+      </c>
+      <c r="BN9" s="2">
+        <v>1453</v>
+      </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -3234,8 +3292,14 @@
       <c r="BL10" s="2">
         <v>1418</v>
       </c>
+      <c r="BM10" s="2">
+        <v>1478</v>
+      </c>
+      <c r="BN10" s="2">
+        <v>1486</v>
+      </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -3428,8 +3492,14 @@
       <c r="BL11" s="2">
         <v>107</v>
       </c>
+      <c r="BM11" s="2">
+        <v>109</v>
+      </c>
+      <c r="BN11" s="2">
+        <v>113</v>
+      </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -3622,8 +3692,14 @@
       <c r="BL12" s="2">
         <v>425</v>
       </c>
+      <c r="BM12" s="2">
+        <v>433</v>
+      </c>
+      <c r="BN12" s="2">
+        <v>436</v>
+      </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -3816,8 +3892,14 @@
       <c r="BL13" s="2">
         <v>2285</v>
       </c>
+      <c r="BM13" s="2">
+        <v>2407</v>
+      </c>
+      <c r="BN13" s="2">
+        <v>2457</v>
+      </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -4010,8 +4092,14 @@
       <c r="BL14" s="2">
         <v>73</v>
       </c>
+      <c r="BM14" s="2">
+        <v>74</v>
+      </c>
+      <c r="BN14" s="2">
+        <v>74</v>
+      </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -4204,8 +4292,14 @@
       <c r="BL15" s="2">
         <v>1734</v>
       </c>
+      <c r="BM15" s="2">
+        <v>2228</v>
+      </c>
+      <c r="BN15" s="2">
+        <v>2228</v>
+      </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -4398,8 +4492,14 @@
       <c r="BL16" s="2">
         <v>22592</v>
       </c>
+      <c r="BM16" s="2">
+        <v>22783</v>
+      </c>
+      <c r="BN16" s="2">
+        <v>23010</v>
+      </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -4592,8 +4692,14 @@
       <c r="BL17" s="2">
         <v>63752</v>
       </c>
+      <c r="BM17" s="2">
+        <v>66467</v>
+      </c>
+      <c r="BN17" s="2">
+        <v>67524</v>
+      </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -4786,8 +4892,14 @@
       <c r="BL18" s="2">
         <v>2044</v>
       </c>
+      <c r="BM18" s="2">
+        <v>2163</v>
+      </c>
+      <c r="BN18" s="2">
+        <v>2202</v>
+      </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -4980,8 +5092,14 @@
       <c r="BL19" s="2">
         <v>2</v>
       </c>
+      <c r="BM19" s="2">
+        <v>2</v>
+      </c>
+      <c r="BN19" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -5174,8 +5292,14 @@
       <c r="BL20" s="2">
         <v>998</v>
       </c>
+      <c r="BM20" s="2">
+        <v>1014</v>
+      </c>
+      <c r="BN20" s="2">
+        <v>1018</v>
+      </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -5368,8 +5492,14 @@
       <c r="BL21" s="2">
         <v>6910</v>
       </c>
+      <c r="BM21" s="2">
+        <v>7004</v>
+      </c>
+      <c r="BN21" s="2">
+        <v>7039</v>
+      </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -5562,8 +5692,14 @@
       <c r="BL22" s="2">
         <v>14138</v>
       </c>
+      <c r="BM22" s="2">
+        <v>14404</v>
+      </c>
+      <c r="BN22" s="2">
+        <v>14458</v>
+      </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
@@ -5756,8 +5892,14 @@
       <c r="BL23" s="2">
         <v>12295</v>
       </c>
+      <c r="BM23" s="2">
+        <v>12620</v>
+      </c>
+      <c r="BN23" s="2">
+        <v>12973</v>
+      </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -5950,8 +6092,14 @@
       <c r="BL24" s="2">
         <v>943</v>
       </c>
+      <c r="BM24" s="2">
+        <v>945</v>
+      </c>
+      <c r="BN24" s="2">
+        <v>946</v>
+      </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
@@ -6144,8 +6292,14 @@
       <c r="BL25" s="2">
         <v>56</v>
       </c>
+      <c r="BM25" s="2">
+        <v>56</v>
+      </c>
+      <c r="BN25" s="2">
+        <v>56</v>
+      </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -6338,8 +6492,14 @@
       <c r="BL26" s="2">
         <v>111</v>
       </c>
+      <c r="BM26" s="2">
+        <v>116</v>
+      </c>
+      <c r="BN26" s="2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -6532,8 +6692,14 @@
       <c r="BL27" s="2">
         <v>1061</v>
       </c>
+      <c r="BM27" s="2">
+        <v>1066</v>
+      </c>
+      <c r="BN27" s="2">
+        <v>1066</v>
+      </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -6726,8 +6892,14 @@
       <c r="BL28" s="2">
         <v>703</v>
       </c>
+      <c r="BM28" s="2">
+        <v>705</v>
+      </c>
+      <c r="BN28" s="2">
+        <v>715</v>
+      </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
@@ -6920,8 +7092,14 @@
       <c r="BL29" s="2">
         <v>1752</v>
       </c>
+      <c r="BM29" s="2">
+        <v>1793</v>
+      </c>
+      <c r="BN29" s="2">
+        <v>1834</v>
+      </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -7114,8 +7292,14 @@
       <c r="BL30" s="2">
         <v>1145</v>
       </c>
+      <c r="BM30" s="2">
+        <v>1205</v>
+      </c>
+      <c r="BN30" s="2">
+        <v>1230</v>
+      </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -7308,8 +7492,14 @@
       <c r="BL31" s="2">
         <v>1013</v>
       </c>
+      <c r="BM31" s="2">
+        <v>1081</v>
+      </c>
+      <c r="BN31" s="2">
+        <v>1108</v>
+      </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>30</v>
       </c>
@@ -7502,8 +7692,14 @@
       <c r="BL32" s="2">
         <v>315</v>
       </c>
+      <c r="BM32" s="2">
+        <v>316</v>
+      </c>
+      <c r="BN32" s="2">
+        <v>316</v>
+      </c>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
@@ -7696,8 +7892,14 @@
       <c r="BL33" s="2">
         <v>13833</v>
       </c>
+      <c r="BM33" s="2">
+        <v>15058</v>
+      </c>
+      <c r="BN33" s="2">
+        <v>15652</v>
+      </c>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
@@ -7890,8 +8092,14 @@
       <c r="BL34" s="2">
         <v>356</v>
       </c>
+      <c r="BM34" s="2">
+        <v>377</v>
+      </c>
+      <c r="BN34" s="2">
+        <v>385</v>
+      </c>
     </row>
-    <row r="35" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>33</v>
       </c>
@@ -8084,8 +8292,14 @@
       <c r="BL35" s="2">
         <v>152</v>
       </c>
+      <c r="BM35" s="2">
+        <v>154</v>
+      </c>
+      <c r="BN35" s="2">
+        <v>154</v>
+      </c>
     </row>
-    <row r="36" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>34</v>
       </c>
@@ -8278,8 +8492,14 @@
       <c r="BL36" s="2">
         <v>778</v>
       </c>
+      <c r="BM36" s="2">
+        <v>792</v>
+      </c>
+      <c r="BN36" s="2">
+        <v>799</v>
+      </c>
     </row>
-    <row r="37" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
@@ -8472,8 +8692,14 @@
       <c r="BL37" s="2">
         <v>318</v>
       </c>
+      <c r="BM37" s="2">
+        <v>324</v>
+      </c>
+      <c r="BN37" s="2">
+        <v>328</v>
+      </c>
     </row>
-    <row r="38" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>36</v>
       </c>
@@ -8666,8 +8892,14 @@
       <c r="BL38" s="2">
         <v>1441</v>
       </c>
+      <c r="BM38" s="2">
+        <v>1456</v>
+      </c>
+      <c r="BN38" s="2">
+        <v>1459</v>
+      </c>
     </row>
-    <row r="39" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
@@ -8860,8 +9092,14 @@
       <c r="BL39" s="2">
         <v>1392</v>
       </c>
+      <c r="BM39" s="2">
+        <v>1422</v>
+      </c>
+      <c r="BN39" s="2">
+        <v>1429</v>
+      </c>
     </row>
-    <row r="40" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>38</v>
       </c>
@@ -9054,8 +9292,14 @@
       <c r="BL40" s="2">
         <v>289</v>
       </c>
+      <c r="BM40" s="2">
+        <v>289</v>
+      </c>
+      <c r="BN40" s="2">
+        <v>289</v>
+      </c>
     </row>
-    <row r="41" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
@@ -9248,8 +9492,14 @@
       <c r="BL41" s="2">
         <v>325</v>
       </c>
+      <c r="BM41" s="2">
+        <v>329</v>
+      </c>
+      <c r="BN41" s="2">
+        <v>331</v>
+      </c>
     </row>
-    <row r="42" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
@@ -9442,8 +9692,14 @@
       <c r="BL42" s="2">
         <v>19</v>
       </c>
+      <c r="BM42" s="2">
+        <v>19</v>
+      </c>
+      <c r="BN42" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="43" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>41</v>
       </c>
@@ -9636,8 +9892,14 @@
       <c r="BL43" s="2">
         <v>36</v>
       </c>
+      <c r="BM43" s="2">
+        <v>36</v>
+      </c>
+      <c r="BN43" s="2">
+        <v>36</v>
+      </c>
     </row>
-    <row r="44" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
@@ -9830,8 +10092,14 @@
       <c r="BL44" s="2">
         <v>190</v>
       </c>
+      <c r="BM44" s="2">
+        <v>191</v>
+      </c>
+      <c r="BN44" s="2">
+        <v>191</v>
+      </c>
     </row>
-    <row r="45" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
@@ -10024,8 +10292,14 @@
       <c r="BL45" s="2">
         <v>39489</v>
       </c>
+      <c r="BM45" s="2">
+        <v>40325</v>
+      </c>
+      <c r="BN45" s="2">
+        <v>40645</v>
+      </c>
     </row>
-    <row r="46" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>44</v>
       </c>
@@ -10218,8 +10492,14 @@
       <c r="BL46" s="2">
         <v>159</v>
       </c>
+      <c r="BM46" s="2">
+        <v>160</v>
+      </c>
+      <c r="BN46" s="2">
+        <v>160</v>
+      </c>
     </row>
-    <row r="47" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
@@ -10412,8 +10692,14 @@
       <c r="BL47" s="2">
         <v>1183</v>
       </c>
+      <c r="BM47" s="2">
+        <v>1207</v>
+      </c>
+      <c r="BN47" s="2">
+        <v>1221</v>
+      </c>
     </row>
-    <row r="48" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>46</v>
       </c>
@@ -10606,8 +10892,14 @@
       <c r="BL48" s="2">
         <v>5302</v>
       </c>
+      <c r="BM48" s="2">
+        <v>5654</v>
+      </c>
+      <c r="BN48" s="2">
+        <v>5905</v>
+      </c>
     </row>
-    <row r="49" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
@@ -10800,8 +11092,14 @@
       <c r="BL49" s="2">
         <v>681</v>
       </c>
+      <c r="BM49" s="2">
+        <v>685</v>
+      </c>
+      <c r="BN49" s="2">
+        <v>685</v>
+      </c>
     </row>
-    <row r="50" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
@@ -10994,8 +11292,14 @@
       <c r="BL50" s="2">
         <v>93</v>
       </c>
+      <c r="BM50" s="2">
+        <v>93</v>
+      </c>
+      <c r="BN50" s="2">
+        <v>93</v>
+      </c>
     </row>
-    <row r="51" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
@@ -11188,8 +11492,14 @@
       <c r="BL51" s="2">
         <v>1607</v>
       </c>
+      <c r="BM51" s="2">
+        <v>1645</v>
+      </c>
+      <c r="BN51" s="2">
+        <v>1653</v>
+      </c>
     </row>
-    <row r="52" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>50</v>
       </c>
@@ -11382,8 +11692,14 @@
       <c r="BL52" s="2">
         <v>6734</v>
       </c>
+      <c r="BM52" s="2">
+        <v>6966</v>
+      </c>
+      <c r="BN52" s="2">
+        <v>6992</v>
+      </c>
     </row>
-    <row r="53" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
@@ -11576,8 +11892,14 @@
       <c r="BL53" s="2">
         <v>37</v>
       </c>
+      <c r="BM53" s="2">
+        <v>37</v>
+      </c>
+      <c r="BN53" s="2">
+        <v>38</v>
+      </c>
     </row>
-    <row r="54" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>52</v>
       </c>
@@ -11770,8 +12092,14 @@
       <c r="BL54" s="2">
         <v>157</v>
       </c>
+      <c r="BM54" s="2">
+        <v>159</v>
+      </c>
+      <c r="BN54" s="2">
+        <v>169</v>
+      </c>
     </row>
-    <row r="55" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -11964,8 +12292,14 @@
       <c r="BL55" s="2">
         <v>109</v>
       </c>
+      <c r="BM55" s="2">
+        <v>109</v>
+      </c>
+      <c r="BN55" s="2">
+        <v>109</v>
+      </c>
     </row>
-    <row r="56" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>54</v>
       </c>
@@ -12158,8 +12492,14 @@
       <c r="BL56" s="2">
         <v>159</v>
       </c>
+      <c r="BM56" s="2">
+        <v>159</v>
+      </c>
+      <c r="BN56" s="2">
+        <v>162</v>
+      </c>
     </row>
-    <row r="57" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>55</v>
       </c>
@@ -12352,8 +12692,14 @@
       <c r="BL57" s="2">
         <v>38</v>
       </c>
+      <c r="BM57" s="2">
+        <v>38</v>
+      </c>
+      <c r="BN57" s="2">
+        <v>38</v>
+      </c>
     </row>
-    <row r="58" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>56</v>
       </c>
@@ -12546,8 +12892,14 @@
       <c r="BL58" s="2">
         <v>10</v>
       </c>
+      <c r="BM58" s="2">
+        <v>10</v>
+      </c>
+      <c r="BN58" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="59" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>57</v>
       </c>
@@ -12740,8 +13092,14 @@
       <c r="BL59" s="2">
         <v>152018</v>
       </c>
+      <c r="BM59" s="2">
+        <v>154855</v>
+      </c>
+      <c r="BN59" s="2">
+        <v>155980</v>
+      </c>
     </row>
-    <row r="60" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
@@ -12934,8 +13292,14 @@
       <c r="BL60" s="2">
         <v>444</v>
       </c>
+      <c r="BM60" s="2">
+        <v>444</v>
+      </c>
+      <c r="BN60" s="2">
+        <v>446</v>
+      </c>
     </row>
-    <row r="61" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>59</v>
       </c>
@@ -13128,8 +13492,14 @@
       <c r="BL61" s="2">
         <v>424</v>
       </c>
+      <c r="BM61" s="2">
+        <v>433</v>
+      </c>
+      <c r="BN61" s="2">
+        <v>435</v>
+      </c>
     </row>
-    <row r="62" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>60</v>
       </c>
@@ -13322,8 +13692,14 @@
       <c r="BL62" s="2">
         <v>101</v>
       </c>
+      <c r="BM62" s="2">
+        <v>106</v>
+      </c>
+      <c r="BN62" s="2">
+        <v>106</v>
+      </c>
     </row>
-    <row r="63" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>61</v>
       </c>
@@ -13516,8 +13892,14 @@
       <c r="BL63" s="2">
         <v>35563</v>
       </c>
+      <c r="BM63" s="2">
+        <v>36387</v>
+      </c>
+      <c r="BN63" s="2">
+        <v>36657</v>
+      </c>
     </row>
-    <row r="64" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>62</v>
       </c>
@@ -13710,8 +14092,14 @@
       <c r="BL64" s="2">
         <v>520</v>
       </c>
+      <c r="BM64" s="2">
+        <v>534</v>
+      </c>
+      <c r="BN64" s="2">
+        <v>546</v>
+      </c>
     </row>
-    <row r="65" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>63</v>
       </c>
@@ -13904,8 +14292,14 @@
       <c r="BL65" s="2">
         <v>26</v>
       </c>
+      <c r="BM65" s="2">
+        <v>26</v>
+      </c>
+      <c r="BN65" s="2">
+        <v>28</v>
+      </c>
     </row>
-    <row r="66" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>64</v>
       </c>
@@ -14098,8 +14492,14 @@
       <c r="BL66" s="2">
         <v>187</v>
       </c>
+      <c r="BM66" s="2">
+        <v>188</v>
+      </c>
+      <c r="BN66" s="2">
+        <v>188</v>
+      </c>
     </row>
-    <row r="67" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>65</v>
       </c>
@@ -14292,8 +14692,14 @@
       <c r="BL67" s="2">
         <v>190</v>
       </c>
+      <c r="BM67" s="2">
+        <v>193</v>
+      </c>
+      <c r="BN67" s="2">
+        <v>193</v>
+      </c>
     </row>
-    <row r="68" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>66</v>
       </c>
@@ -14486,8 +14892,14 @@
       <c r="BL68" s="2">
         <v>386</v>
       </c>
+      <c r="BM68" s="2">
+        <v>393</v>
+      </c>
+      <c r="BN68" s="2">
+        <v>393</v>
+      </c>
     </row>
-    <row r="69" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>67</v>
       </c>
@@ -14680,8 +15092,14 @@
       <c r="BL69" s="2">
         <v>419</v>
       </c>
+      <c r="BM69" s="2">
+        <v>421</v>
+      </c>
+      <c r="BN69" s="2">
+        <v>421</v>
+      </c>
     </row>
-    <row r="70" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>68</v>
       </c>
@@ -14874,8 +15292,14 @@
       <c r="BL70" s="2">
         <v>4712</v>
       </c>
+      <c r="BM70" s="2">
+        <v>4929</v>
+      </c>
+      <c r="BN70" s="2">
+        <v>5101</v>
+      </c>
     </row>
-    <row r="71" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>69</v>
       </c>
@@ -15068,8 +15492,14 @@
       <c r="BL71" s="2">
         <v>31</v>
       </c>
+      <c r="BM71" s="2">
+        <v>32</v>
+      </c>
+      <c r="BN71" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="72" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>70</v>
       </c>
@@ -15262,8 +15692,14 @@
       <c r="BL72" s="2">
         <v>9005</v>
       </c>
+      <c r="BM72" s="2">
+        <v>9176</v>
+      </c>
+      <c r="BN72" s="2">
+        <v>9202</v>
+      </c>
     </row>
-    <row r="73" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>71</v>
       </c>
@@ -15456,8 +15892,14 @@
       <c r="BL73" s="2">
         <v>44256</v>
       </c>
+      <c r="BM73" s="2">
+        <v>44534</v>
+      </c>
+      <c r="BN73" s="2">
+        <v>44566</v>
+      </c>
     </row>
-    <row r="74" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>72</v>
       </c>
@@ -15650,8 +16092,14 @@
       <c r="BL74" s="2">
         <v>1516</v>
       </c>
+      <c r="BM74" s="2">
+        <v>1525</v>
+      </c>
+      <c r="BN74" s="2">
+        <v>1526</v>
+      </c>
     </row>
-    <row r="75" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>73</v>
       </c>
@@ -15844,8 +16292,14 @@
       <c r="BL75" s="2">
         <v>847</v>
       </c>
+      <c r="BM75" s="2">
+        <v>853</v>
+      </c>
+      <c r="BN75" s="2">
+        <v>857</v>
+      </c>
     </row>
-    <row r="76" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>74</v>
       </c>
@@ -16038,8 +16492,14 @@
       <c r="BL76" s="2">
         <v>1432</v>
       </c>
+      <c r="BM76" s="2">
+        <v>1451</v>
+      </c>
+      <c r="BN76" s="2">
+        <v>1454</v>
+      </c>
     </row>
-    <row r="77" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>75</v>
       </c>
@@ -16232,8 +16692,14 @@
       <c r="BL77" s="2">
         <v>1466</v>
       </c>
+      <c r="BM77" s="2">
+        <v>1503</v>
+      </c>
+      <c r="BN77" s="2">
+        <v>1522</v>
+      </c>
     </row>
-    <row r="78" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>76</v>
       </c>
@@ -16426,8 +16892,14 @@
       <c r="BL78" s="2">
         <v>32</v>
       </c>
+      <c r="BM78" s="2">
+        <v>32</v>
+      </c>
+      <c r="BN78" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="79" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>77</v>
       </c>
@@ -16620,8 +17092,14 @@
       <c r="BL79" s="2">
         <v>279</v>
       </c>
+      <c r="BM79" s="2">
+        <v>279</v>
+      </c>
+      <c r="BN79" s="2">
+        <v>280</v>
+      </c>
     </row>
-    <row r="80" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>78</v>
       </c>
@@ -16814,8 +17292,14 @@
       <c r="BL80" s="2">
         <v>96</v>
       </c>
+      <c r="BM80" s="2">
+        <v>96</v>
+      </c>
+      <c r="BN80" s="2">
+        <v>96</v>
+      </c>
     </row>
-    <row r="81" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>79</v>
       </c>
@@ -17008,8 +17492,14 @@
       <c r="BL81" s="2">
         <v>89616</v>
       </c>
+      <c r="BM81" s="2">
+        <v>92332</v>
+      </c>
+      <c r="BN81" s="2">
+        <v>93506</v>
+      </c>
     </row>
-    <row r="82" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>80</v>
       </c>
@@ -17202,8 +17692,14 @@
       <c r="BL82" s="2">
         <v>262</v>
       </c>
+      <c r="BM82" s="2">
+        <v>271</v>
+      </c>
+      <c r="BN82" s="2">
+        <v>276</v>
+      </c>
     </row>
-    <row r="83" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>81</v>
       </c>
@@ -17396,8 +17892,14 @@
       <c r="BL83" s="2">
         <v>680</v>
       </c>
+      <c r="BM83" s="2">
+        <v>688</v>
+      </c>
+      <c r="BN83" s="2">
+        <v>689</v>
+      </c>
     </row>
-    <row r="84" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>82</v>
       </c>
@@ -17590,8 +18092,14 @@
       <c r="BL84" s="2">
         <v>748</v>
       </c>
+      <c r="BM84" s="2">
+        <v>751</v>
+      </c>
+      <c r="BN84" s="2">
+        <v>758</v>
+      </c>
     </row>
-    <row r="85" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>83</v>
       </c>
@@ -17784,8 +18292,14 @@
       <c r="BL85" s="2">
         <v>275</v>
       </c>
+      <c r="BM85" s="2">
+        <v>277</v>
+      </c>
+      <c r="BN85" s="2">
+        <v>280</v>
+      </c>
     </row>
-    <row r="86" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>84</v>
       </c>
@@ -17978,8 +18492,14 @@
       <c r="BL86" s="2">
         <v>38251</v>
       </c>
+      <c r="BM86" s="2">
+        <v>38645</v>
+      </c>
+      <c r="BN86" s="2">
+        <v>38917</v>
+      </c>
     </row>
-    <row r="87" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -18172,8 +18692,14 @@
       <c r="BL87" s="2">
         <v>3</v>
       </c>
+      <c r="BM87" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN87" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="88" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>86</v>
       </c>
@@ -18366,8 +18892,14 @@
       <c r="BL88" s="2">
         <v>1005</v>
       </c>
+      <c r="BM88" s="2">
+        <v>1100</v>
+      </c>
+      <c r="BN88" s="2">
+        <v>1158</v>
+      </c>
     </row>
-    <row r="89" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>87</v>
       </c>
@@ -18560,8 +19092,14 @@
       <c r="BL89" s="2">
         <v>72</v>
       </c>
+      <c r="BM89" s="2">
+        <v>76</v>
+      </c>
+      <c r="BN89" s="2">
+        <v>76</v>
+      </c>
     </row>
-    <row r="90" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>88</v>
       </c>
@@ -18754,8 +19292,14 @@
       <c r="BL90" s="2">
         <v>177</v>
       </c>
+      <c r="BM90" s="2">
+        <v>178</v>
+      </c>
+      <c r="BN90" s="2">
+        <v>181</v>
+      </c>
     </row>
-    <row r="91" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>89</v>
       </c>
@@ -18948,8 +19492,14 @@
       <c r="BL91" s="2">
         <v>1091</v>
       </c>
+      <c r="BM91" s="2">
+        <v>1117</v>
+      </c>
+      <c r="BN91" s="2">
+        <v>1118</v>
+      </c>
     </row>
-    <row r="92" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>90</v>
       </c>
@@ -19142,8 +19692,14 @@
       <c r="BL92" s="2">
         <v>862</v>
       </c>
+      <c r="BM92" s="2">
+        <v>874</v>
+      </c>
+      <c r="BN92" s="2">
+        <v>876</v>
+      </c>
     </row>
-    <row r="93" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>91</v>
       </c>
@@ -19336,8 +19892,14 @@
       <c r="BL93" s="2">
         <v>7378</v>
       </c>
+      <c r="BM93" s="2">
+        <v>7487</v>
+      </c>
+      <c r="BN93" s="2">
+        <v>7520</v>
+      </c>
     </row>
-    <row r="94" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>92</v>
       </c>
@@ -19530,8 +20092,14 @@
       <c r="BL94" s="2">
         <v>3027</v>
       </c>
+      <c r="BM94" s="2">
+        <v>3067</v>
+      </c>
+      <c r="BN94" s="2">
+        <v>3105</v>
+      </c>
     </row>
-    <row r="95" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>93</v>
       </c>
@@ -19724,8 +20292,14 @@
       <c r="BL95" s="2">
         <v>1106</v>
       </c>
+      <c r="BM95" s="2">
+        <v>1115</v>
+      </c>
+      <c r="BN95" s="2">
+        <v>1127</v>
+      </c>
     </row>
-    <row r="96" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>94</v>
       </c>
@@ -19918,8 +20492,14 @@
       <c r="BL96" s="2">
         <v>3736</v>
       </c>
+      <c r="BM96" s="2">
+        <v>3976</v>
+      </c>
+      <c r="BN96" s="2">
+        <v>4091</v>
+      </c>
     </row>
-    <row r="97" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>95</v>
       </c>
@@ -20112,8 +20692,14 @@
       <c r="BL97" s="2">
         <v>436</v>
       </c>
+      <c r="BM97" s="2">
+        <v>451</v>
+      </c>
+      <c r="BN97" s="2">
+        <v>459</v>
+      </c>
     </row>
-    <row r="98" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>96</v>
       </c>
@@ -20306,8 +20892,14 @@
       <c r="BL98" s="2">
         <v>161</v>
       </c>
+      <c r="BM98" s="2">
+        <v>163</v>
+      </c>
+      <c r="BN98" s="2">
+        <v>163</v>
+      </c>
     </row>
-    <row r="99" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>97</v>
       </c>
@@ -20500,8 +21092,14 @@
       <c r="BL99" s="2">
         <v>784</v>
       </c>
+      <c r="BM99" s="2">
+        <v>815</v>
+      </c>
+      <c r="BN99" s="2">
+        <v>816</v>
+      </c>
     </row>
-    <row r="100" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>98</v>
       </c>
@@ -20694,8 +21292,14 @@
       <c r="BL100" s="2">
         <v>55</v>
       </c>
+      <c r="BM100" s="2">
+        <v>56</v>
+      </c>
+      <c r="BN100" s="2">
+        <v>58</v>
+      </c>
     </row>
-    <row r="101" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>99</v>
       </c>
@@ -20888,8 +21492,14 @@
       <c r="BL101" s="2">
         <v>60</v>
       </c>
+      <c r="BM101" s="2">
+        <v>60</v>
+      </c>
+      <c r="BN101" s="2">
+        <v>60</v>
+      </c>
     </row>
-    <row r="102" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>100</v>
       </c>
@@ -21082,8 +21692,14 @@
       <c r="BL102" s="2">
         <v>903</v>
       </c>
+      <c r="BM102" s="2">
+        <v>913</v>
+      </c>
+      <c r="BN102" s="2">
+        <v>914</v>
+      </c>
     </row>
-    <row r="103" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>101</v>
       </c>
@@ -21276,8 +21892,14 @@
       <c r="BL103" s="2">
         <v>257823</v>
       </c>
+      <c r="BM103" s="2">
+        <v>261127</v>
+      </c>
+      <c r="BN103" s="2">
+        <v>261461</v>
+      </c>
     </row>
-    <row r="104" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>102</v>
       </c>
@@ -21470,8 +22092,14 @@
       <c r="BL104" s="2">
         <v>4654</v>
       </c>
+      <c r="BM104" s="2">
+        <v>4704</v>
+      </c>
+      <c r="BN104" s="2">
+        <v>4739</v>
+      </c>
     </row>
-    <row r="105" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>103</v>
       </c>
@@ -21664,8 +22292,14 @@
       <c r="BL105" s="2">
         <v>89</v>
       </c>
+      <c r="BM105" s="2">
+        <v>90</v>
+      </c>
+      <c r="BN105" s="2">
+        <v>90</v>
+      </c>
     </row>
-    <row r="106" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>104</v>
       </c>
@@ -21858,8 +22492,14 @@
       <c r="BL106" s="2">
         <v>286</v>
       </c>
+      <c r="BM106" s="2">
+        <v>286</v>
+      </c>
+      <c r="BN106" s="2">
+        <v>286</v>
+      </c>
     </row>
-    <row r="107" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>105</v>
       </c>
@@ -22052,8 +22692,14 @@
       <c r="BL107" s="2">
         <v>10923</v>
       </c>
+      <c r="BM107" s="2">
+        <v>11651</v>
+      </c>
+      <c r="BN107" s="2">
+        <v>11968</v>
+      </c>
     </row>
-    <row r="108" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>106</v>
       </c>
@@ -22246,8 +22892,14 @@
       <c r="BL108" s="2">
         <v>182</v>
       </c>
+      <c r="BM108" s="2">
+        <v>183</v>
+      </c>
+      <c r="BN108" s="2">
+        <v>183</v>
+      </c>
     </row>
-    <row r="109" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>107</v>
       </c>
@@ -22440,8 +23092,14 @@
       <c r="BL109" s="2">
         <v>1959</v>
       </c>
+      <c r="BM109" s="2">
+        <v>2006</v>
+      </c>
+      <c r="BN109" s="2">
+        <v>2013</v>
+      </c>
     </row>
-    <row r="110" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>108</v>
       </c>
@@ -22634,8 +23292,14 @@
       <c r="BL110" s="2">
         <v>23699</v>
       </c>
+      <c r="BM110" s="2">
+        <v>24720</v>
+      </c>
+      <c r="BN110" s="2">
+        <v>24992</v>
+      </c>
     </row>
-    <row r="111" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>109</v>
       </c>
@@ -22828,8 +23492,14 @@
       <c r="BL111" s="2">
         <v>1267</v>
       </c>
+      <c r="BM111" s="2">
+        <v>1301</v>
+      </c>
+      <c r="BN111" s="2">
+        <v>1312</v>
+      </c>
     </row>
-    <row r="112" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>110</v>
       </c>
@@ -23022,8 +23692,14 @@
       <c r="BL112" s="2">
         <v>94</v>
       </c>
+      <c r="BM112" s="2">
+        <v>96</v>
+      </c>
+      <c r="BN112" s="2">
+        <v>105</v>
+      </c>
     </row>
-    <row r="113" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>111</v>
       </c>
@@ -23216,8 +23892,14 @@
       <c r="BL113" s="2">
         <v>1227</v>
       </c>
+      <c r="BM113" s="2">
+        <v>1232</v>
+      </c>
+      <c r="BN113" s="2">
+        <v>1233</v>
+      </c>
     </row>
-    <row r="114" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>112</v>
       </c>
@@ -23410,8 +24092,14 @@
       <c r="BL114" s="2">
         <v>721</v>
       </c>
+      <c r="BM114" s="2">
+        <v>737</v>
+      </c>
+      <c r="BN114" s="2">
+        <v>738</v>
+      </c>
     </row>
-    <row r="115" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>113</v>
       </c>
@@ -23604,8 +24292,14 @@
       <c r="BL115" s="2">
         <v>1588</v>
       </c>
+      <c r="BM115" s="2">
+        <v>1709</v>
+      </c>
+      <c r="BN115" s="2">
+        <v>1715</v>
+      </c>
     </row>
-    <row r="116" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>114</v>
       </c>
@@ -23798,8 +24492,14 @@
       <c r="BL116" s="2">
         <v>399</v>
       </c>
+      <c r="BM116" s="2">
+        <v>416</v>
+      </c>
+      <c r="BN116" s="2">
+        <v>454</v>
+      </c>
     </row>
-    <row r="117" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>115</v>
       </c>
@@ -23992,8 +24692,14 @@
       <c r="BL117" s="2">
         <v>58</v>
       </c>
+      <c r="BM117" s="2">
+        <v>58</v>
+      </c>
+      <c r="BN117" s="2">
+        <v>58</v>
+      </c>
     </row>
-    <row r="118" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>116</v>
       </c>
@@ -24186,8 +24892,14 @@
       <c r="BL118" s="2">
         <v>3903</v>
       </c>
+      <c r="BM118" s="2">
+        <v>3936</v>
+      </c>
+      <c r="BN118" s="2">
+        <v>3946</v>
+      </c>
     </row>
-    <row r="119" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>117</v>
       </c>
@@ -24380,8 +25092,14 @@
       <c r="BL119" s="2">
         <v>637</v>
       </c>
+      <c r="BM119" s="2">
+        <v>648</v>
+      </c>
+      <c r="BN119" s="2">
+        <v>649</v>
+      </c>
     </row>
-    <row r="120" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>118</v>
       </c>
@@ -24574,8 +25292,14 @@
       <c r="BL120" s="2">
         <v>6</v>
       </c>
+      <c r="BM120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BN120" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="121" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>119</v>
       </c>
@@ -24768,8 +25492,14 @@
       <c r="BL121" s="2">
         <v>106</v>
       </c>
+      <c r="BM121" s="2">
+        <v>107</v>
+      </c>
+      <c r="BN121" s="2">
+        <v>107</v>
+      </c>
     </row>
-    <row r="122" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>120</v>
       </c>
@@ -24962,8 +25692,14 @@
       <c r="BL122" s="2">
         <v>884</v>
       </c>
+      <c r="BM122" s="2">
+        <v>892</v>
+      </c>
+      <c r="BN122" s="2">
+        <v>901</v>
+      </c>
     </row>
-    <row r="123" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>121</v>
       </c>
@@ -25156,8 +25892,14 @@
       <c r="BL123" s="2">
         <v>869</v>
       </c>
+      <c r="BM123" s="2">
+        <v>880</v>
+      </c>
+      <c r="BN123" s="2">
+        <v>884</v>
+      </c>
     </row>
-    <row r="124" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>122</v>
       </c>
@@ -25350,8 +26092,14 @@
       <c r="BL124" s="2">
         <v>11</v>
       </c>
+      <c r="BM124" s="2">
+        <v>11</v>
+      </c>
+      <c r="BN124" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="125" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>123</v>
       </c>
@@ -25544,8 +26292,14 @@
       <c r="BL125" s="2">
         <v>15052</v>
       </c>
+      <c r="BM125" s="2">
+        <v>15609</v>
+      </c>
+      <c r="BN125" s="2">
+        <v>15984</v>
+      </c>
     </row>
-    <row r="126" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>124</v>
       </c>
@@ -25738,8 +26492,14 @@
       <c r="BL126" s="2">
         <v>132</v>
       </c>
+      <c r="BM126" s="2">
+        <v>133</v>
+      </c>
+      <c r="BN126" s="2">
+        <v>133</v>
+      </c>
     </row>
-    <row r="127" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>125</v>
       </c>
@@ -25932,8 +26692,14 @@
       <c r="BL127" s="2">
         <v>2211</v>
       </c>
+      <c r="BM127" s="2">
+        <v>2235</v>
+      </c>
+      <c r="BN127" s="2">
+        <v>2235</v>
+      </c>
     </row>
-    <row r="128" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
         <v>126</v>
       </c>
@@ -26126,8 +26892,14 @@
       <c r="BL128" s="2">
         <v>8010</v>
       </c>
+      <c r="BM128" s="2">
+        <v>8159</v>
+      </c>
+      <c r="BN128" s="2">
+        <v>8198</v>
+      </c>
     </row>
-    <row r="129" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>127</v>
       </c>
@@ -26320,8 +27092,14 @@
       <c r="BL129" s="2">
         <v>605</v>
       </c>
+      <c r="BM129" s="2">
+        <v>616</v>
+      </c>
+      <c r="BN129" s="2">
+        <v>616</v>
+      </c>
     </row>
-    <row r="130" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
         <v>128</v>
       </c>
@@ -26514,8 +27292,14 @@
       <c r="BL130" s="2">
         <v>322</v>
       </c>
+      <c r="BM130" s="2">
+        <v>326</v>
+      </c>
+      <c r="BN130" s="2">
+        <v>326</v>
+      </c>
     </row>
-    <row r="131" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>129</v>
       </c>
@@ -26708,8 +27492,14 @@
       <c r="BL131" s="2">
         <v>4649</v>
       </c>
+      <c r="BM131" s="2">
+        <v>4708</v>
+      </c>
+      <c r="BN131" s="2">
+        <v>4714</v>
+      </c>
     </row>
-    <row r="132" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
         <v>130</v>
       </c>
@@ -26902,8 +27692,14 @@
       <c r="BL132" s="2">
         <v>1296</v>
       </c>
+      <c r="BM132" s="2">
+        <v>1321</v>
+      </c>
+      <c r="BN132" s="2">
+        <v>1332</v>
+      </c>
     </row>
-    <row r="133" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>131</v>
       </c>
@@ -27096,8 +27892,14 @@
       <c r="BL133" s="2">
         <v>3</v>
       </c>
+      <c r="BM133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN133" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="134" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>132</v>
       </c>
@@ -27290,8 +28092,14 @@
       <c r="BL134" s="2">
         <v>3</v>
       </c>
+      <c r="BM134" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN134" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="135" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>133</v>
       </c>
@@ -27484,8 +28292,14 @@
       <c r="BL135" s="2">
         <v>2293</v>
       </c>
+      <c r="BM135" s="2">
+        <v>2582</v>
+      </c>
+      <c r="BN135" s="2">
+        <v>2622</v>
+      </c>
     </row>
-    <row r="136" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
         <v>134</v>
       </c>
@@ -27678,8 +28492,14 @@
       <c r="BL136" s="2">
         <v>130</v>
       </c>
+      <c r="BM136" s="2">
+        <v>130</v>
+      </c>
+      <c r="BN136" s="2">
+        <v>131</v>
+      </c>
     </row>
-    <row r="137" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>135</v>
       </c>
@@ -27872,8 +28692,14 @@
       <c r="BL137" s="2">
         <v>4</v>
       </c>
+      <c r="BM137" s="2">
+        <v>4</v>
+      </c>
+      <c r="BN137" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="138" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
         <v>136</v>
       </c>
@@ -28066,8 +28892,14 @@
       <c r="BL138" s="2">
         <v>23</v>
       </c>
+      <c r="BM138" s="2">
+        <v>23</v>
+      </c>
+      <c r="BN138" s="2">
+        <v>23</v>
+      </c>
     </row>
-    <row r="139" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>137</v>
       </c>
@@ -28260,8 +29092,14 @@
       <c r="BL139" s="2">
         <v>2343</v>
       </c>
+      <c r="BM139" s="2">
+        <v>2388</v>
+      </c>
+      <c r="BN139" s="2">
+        <v>2389</v>
+      </c>
     </row>
-    <row r="140" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>138</v>
       </c>
@@ -28454,8 +29292,14 @@
       <c r="BL140" s="2">
         <v>210</v>
       </c>
+      <c r="BM140" s="2">
+        <v>210</v>
+      </c>
+      <c r="BN140" s="2">
+        <v>209</v>
+      </c>
     </row>
-    <row r="141" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>139</v>
       </c>
@@ -28648,8 +29492,14 @@
       <c r="BL141" s="2">
         <v>1361</v>
       </c>
+      <c r="BM141" s="2">
+        <v>1388</v>
+      </c>
+      <c r="BN141" s="2">
+        <v>1393</v>
+      </c>
     </row>
-    <row r="142" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
         <v>140</v>
       </c>
@@ -28842,8 +29692,14 @@
       <c r="BL142" s="2">
         <v>216</v>
       </c>
+      <c r="BM142" s="2">
+        <v>216</v>
+      </c>
+      <c r="BN142" s="2">
+        <v>216</v>
+      </c>
     </row>
-    <row r="143" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
         <v>141</v>
       </c>
@@ -29036,8 +29892,14 @@
       <c r="BL143" s="2">
         <v>1536</v>
       </c>
+      <c r="BM143" s="2">
+        <v>1541</v>
+      </c>
+      <c r="BN143" s="2">
+        <v>1554</v>
+      </c>
     </row>
-    <row r="144" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
         <v>142</v>
       </c>
@@ -29230,8 +30092,14 @@
       <c r="BL144" s="2">
         <v>529</v>
       </c>
+      <c r="BM144" s="2">
+        <v>532</v>
+      </c>
+      <c r="BN144" s="2">
+        <v>537</v>
+      </c>
     </row>
-    <row r="145" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
         <v>143</v>
       </c>
@@ -29424,8 +30292,14 @@
       <c r="BL145" s="2">
         <v>677</v>
       </c>
+      <c r="BM145" s="2">
+        <v>711</v>
+      </c>
+      <c r="BN145" s="2">
+        <v>726</v>
+      </c>
     </row>
-    <row r="146" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
         <v>144</v>
       </c>
@@ -29618,8 +30492,14 @@
       <c r="BL146" s="2">
         <v>369</v>
       </c>
+      <c r="BM146" s="2">
+        <v>375</v>
+      </c>
+      <c r="BN146" s="2">
+        <v>378</v>
+      </c>
     </row>
-    <row r="147" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
         <v>145</v>
       </c>
@@ -29812,8 +30692,14 @@
       <c r="BL147" s="2">
         <v>569</v>
       </c>
+      <c r="BM147" s="2">
+        <v>582</v>
+      </c>
+      <c r="BN147" s="2">
+        <v>595</v>
+      </c>
     </row>
-    <row r="148" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>146</v>
       </c>
@@ -30006,8 +30892,14 @@
       <c r="BL148" s="2">
         <v>3438</v>
       </c>
+      <c r="BM148" s="2">
+        <v>3499</v>
+      </c>
+      <c r="BN148" s="2">
+        <v>3502</v>
+      </c>
     </row>
-    <row r="149" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>147</v>
       </c>
@@ -30200,8 +31092,14 @@
       <c r="BL149" s="2">
         <v>923</v>
       </c>
+      <c r="BM149" s="2">
+        <v>929</v>
+      </c>
+      <c r="BN149" s="2">
+        <v>934</v>
+      </c>
     </row>
-    <row r="150" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>148</v>
       </c>
@@ -30394,8 +31292,14 @@
       <c r="BL150" s="2">
         <v>120</v>
       </c>
+      <c r="BM150" s="2">
+        <v>121</v>
+      </c>
+      <c r="BN150" s="2">
+        <v>121</v>
+      </c>
     </row>
-    <row r="151" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
         <v>149</v>
       </c>
@@ -30588,8 +31492,14 @@
       <c r="BL151" s="2">
         <v>391</v>
       </c>
+      <c r="BM151" s="2">
+        <v>411</v>
+      </c>
+      <c r="BN151" s="2">
+        <v>411</v>
+      </c>
     </row>
-    <row r="152" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>150</v>
       </c>
@@ -30782,8 +31692,14 @@
       <c r="BL152" s="2">
         <v>1149</v>
       </c>
+      <c r="BM152" s="2">
+        <v>1162</v>
+      </c>
+      <c r="BN152" s="2">
+        <v>1172</v>
+      </c>
     </row>
-    <row r="153" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
         <v>151</v>
       </c>
@@ -30976,8 +31892,14 @@
       <c r="BL153" s="2">
         <v>1</v>
       </c>
+      <c r="BM153" s="2">
+        <v>1</v>
+      </c>
+      <c r="BN153" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="154" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>152</v>
       </c>
@@ -31170,8 +32092,14 @@
       <c r="BL154" s="2">
         <v>13101</v>
       </c>
+      <c r="BM154" s="2">
+        <v>13890</v>
+      </c>
+      <c r="BN154" s="2">
+        <v>14449</v>
+      </c>
     </row>
-    <row r="155" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
         <v>153</v>
       </c>
@@ -31364,8 +32292,14 @@
       <c r="BL155" s="2">
         <v>475</v>
       </c>
+      <c r="BM155" s="2">
+        <v>487</v>
+      </c>
+      <c r="BN155" s="2">
+        <v>507</v>
+      </c>
     </row>
-    <row r="156" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>154</v>
       </c>
@@ -31558,8 +32492,14 @@
       <c r="BL156" s="2">
         <v>92</v>
       </c>
+      <c r="BM156" s="2">
+        <v>93</v>
+      </c>
+      <c r="BN156" s="2">
+        <v>93</v>
+      </c>
     </row>
-    <row r="157" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
         <v>155</v>
       </c>
@@ -31752,8 +32692,14 @@
       <c r="BL157" s="2">
         <v>13407</v>
       </c>
+      <c r="BM157" s="2">
+        <v>13729</v>
+      </c>
+      <c r="BN157" s="2">
+        <v>13896</v>
+      </c>
     </row>
-    <row r="158" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>156</v>
       </c>
@@ -31946,8 +32892,14 @@
       <c r="BL158" s="2">
         <v>11</v>
       </c>
+      <c r="BM158" s="2">
+        <v>11</v>
+      </c>
+      <c r="BN158" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="159" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
         <v>157</v>
       </c>
@@ -32140,8 +33092,14 @@
       <c r="BL159" s="2">
         <v>582</v>
       </c>
+      <c r="BM159" s="2">
+        <v>584</v>
+      </c>
+      <c r="BN159" s="2">
+        <v>587</v>
+      </c>
     </row>
-    <row r="160" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>158</v>
       </c>
@@ -32334,8 +33292,14 @@
       <c r="BL160" s="2">
         <v>105</v>
       </c>
+      <c r="BM160" s="2">
+        <v>119</v>
+      </c>
+      <c r="BN160" s="2">
+        <v>122</v>
+      </c>
     </row>
-    <row r="161" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
         <v>159</v>
       </c>
@@ -32528,8 +33492,14 @@
       <c r="BL161" s="2">
         <v>110</v>
       </c>
+      <c r="BM161" s="2">
+        <v>116</v>
+      </c>
+      <c r="BN161" s="2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="162" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>160</v>
       </c>
@@ -32722,8 +33692,14 @@
       <c r="BL162" s="2">
         <v>353</v>
       </c>
+      <c r="BM162" s="2">
+        <v>360</v>
+      </c>
+      <c r="BN162" s="2">
+        <v>362</v>
+      </c>
     </row>
-    <row r="163" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
         <v>161</v>
       </c>
@@ -32916,8 +33892,14 @@
       <c r="BL163" s="2">
         <v>1667</v>
       </c>
+      <c r="BM163" s="2">
+        <v>1680</v>
+      </c>
+      <c r="BN163" s="2">
+        <v>1684</v>
+      </c>
     </row>
-    <row r="164" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
         <v>162</v>
       </c>
@@ -33110,8 +34092,14 @@
       <c r="BL164" s="2">
         <v>3408</v>
       </c>
+      <c r="BM164" s="2">
+        <v>3431</v>
+      </c>
+      <c r="BN164" s="2">
+        <v>3435</v>
+      </c>
     </row>
-    <row r="165" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
         <v>163</v>
       </c>
@@ -33304,8 +34292,14 @@
       <c r="BL165" s="2">
         <v>1135</v>
       </c>
+      <c r="BM165" s="2">
+        <v>1550</v>
+      </c>
+      <c r="BN165" s="2">
+        <v>1562</v>
+      </c>
     </row>
-    <row r="166" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
         <v>164</v>
       </c>
@@ -33498,8 +34492,14 @@
       <c r="BL166" s="2">
         <v>31</v>
       </c>
+      <c r="BM166" s="2">
+        <v>31</v>
+      </c>
+      <c r="BN166" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="167" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
         <v>165</v>
       </c>
@@ -33692,8 +34692,14 @@
       <c r="BL167" s="2">
         <v>5273</v>
       </c>
+      <c r="BM167" s="2">
+        <v>5436</v>
+      </c>
+      <c r="BN167" s="2">
+        <v>5489</v>
+      </c>
     </row>
-    <row r="168" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
         <v>166</v>
       </c>
@@ -33886,8 +34892,14 @@
       <c r="BL168" s="2">
         <v>1630</v>
       </c>
+      <c r="BM168" s="2">
+        <v>1633</v>
+      </c>
+      <c r="BN168" s="2">
+        <v>1646</v>
+      </c>
     </row>
-    <row r="169" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
         <v>167</v>
       </c>
@@ -34080,8 +35092,14 @@
       <c r="BL169" s="2">
         <v>108</v>
       </c>
+      <c r="BM169" s="2">
+        <v>108</v>
+      </c>
+      <c r="BN169" s="2">
+        <v>109</v>
+      </c>
     </row>
-    <row r="170" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
         <v>168</v>
       </c>
@@ -34274,8 +35292,14 @@
       <c r="BL170" s="2">
         <v>226</v>
       </c>
+      <c r="BM170" s="2">
+        <v>228</v>
+      </c>
+      <c r="BN170" s="2">
+        <v>228</v>
+      </c>
     </row>
-    <row r="171" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
         <v>169</v>
       </c>
@@ -34468,8 +35492,14 @@
       <c r="BL171" s="2">
         <v>326</v>
       </c>
+      <c r="BM171" s="2">
+        <v>327</v>
+      </c>
+      <c r="BN171" s="2">
+        <v>327</v>
+      </c>
     </row>
-    <row r="172" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
         <v>170</v>
       </c>
@@ -34662,8 +35692,14 @@
       <c r="BL172" s="2">
         <v>26283</v>
       </c>
+      <c r="BM172" s="2">
+        <v>26785</v>
+      </c>
+      <c r="BN172" s="2">
+        <v>26800</v>
+      </c>
     </row>
-    <row r="173" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>171</v>
       </c>
@@ -34856,8 +35892,14 @@
       <c r="BL173" s="2">
         <v>2904</v>
       </c>
+      <c r="BM173" s="2">
+        <v>2911</v>
+      </c>
+      <c r="BN173" s="2">
+        <v>2912</v>
+      </c>
     </row>
-    <row r="174" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
         <v>172</v>
       </c>
@@ -35050,8 +36092,14 @@
       <c r="BL174" s="2">
         <v>238</v>
       </c>
+      <c r="BM174" s="2">
+        <v>249</v>
+      </c>
+      <c r="BN174" s="2">
+        <v>254</v>
+      </c>
     </row>
-    <row r="175" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
         <v>173</v>
       </c>
@@ -35244,8 +36292,14 @@
       <c r="BL175" s="2">
         <v>27</v>
       </c>
+      <c r="BM175" s="2">
+        <v>28</v>
+      </c>
+      <c r="BN175" s="2">
+        <v>29</v>
+      </c>
     </row>
-    <row r="176" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
         <v>174</v>
       </c>
@@ -35438,8 +36492,14 @@
       <c r="BL176" s="2">
         <v>2954</v>
       </c>
+      <c r="BM176" s="2">
+        <v>3064</v>
+      </c>
+      <c r="BN176" s="2">
+        <v>3088</v>
+      </c>
     </row>
-    <row r="177" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
         <v>175</v>
       </c>
@@ -35632,8 +36692,14 @@
       <c r="BL177" s="2">
         <v>1684</v>
       </c>
+      <c r="BM177" s="2">
+        <v>1728</v>
+      </c>
+      <c r="BN177" s="2">
+        <v>1734</v>
+      </c>
     </row>
-    <row r="178" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
         <v>176</v>
       </c>
@@ -35826,8 +36892,14 @@
       <c r="BL178" s="2">
         <v>315</v>
       </c>
+      <c r="BM178" s="2">
+        <v>317</v>
+      </c>
+      <c r="BN178" s="2">
+        <v>317</v>
+      </c>
     </row>
-    <row r="179" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>177</v>
       </c>
@@ -36020,8 +37092,14 @@
       <c r="BL179" s="2">
         <v>161</v>
       </c>
+      <c r="BM179" s="2">
+        <v>162</v>
+      </c>
+      <c r="BN179" s="2">
+        <v>164</v>
+      </c>
     </row>
-    <row r="180" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
         <v>178</v>
       </c>
@@ -36214,8 +37292,14 @@
       <c r="BL180" s="2">
         <v>6378</v>
       </c>
+      <c r="BM180" s="2">
+        <v>6729</v>
+      </c>
+      <c r="BN180" s="2">
+        <v>6735</v>
+      </c>
     </row>
-    <row r="181" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>179</v>
       </c>
@@ -36408,8 +37492,14 @@
       <c r="BL181" s="2">
         <v>145</v>
       </c>
+      <c r="BM181" s="2">
+        <v>147</v>
+      </c>
+      <c r="BN181" s="2">
+        <v>147</v>
+      </c>
     </row>
-    <row r="182" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
         <v>180</v>
       </c>
@@ -36602,8 +37692,14 @@
       <c r="BL182" s="2">
         <v>113</v>
       </c>
+      <c r="BM182" s="2">
+        <v>115</v>
+      </c>
+      <c r="BN182" s="2">
+        <v>115</v>
+      </c>
     </row>
-    <row r="183" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>181</v>
       </c>
@@ -36796,8 +37892,14 @@
       <c r="BL183" s="2">
         <v>1545</v>
       </c>
+      <c r="BM183" s="2">
+        <v>1576</v>
+      </c>
+      <c r="BN183" s="2">
+        <v>1578</v>
+      </c>
     </row>
-    <row r="184" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>182</v>
       </c>
@@ -36990,8 +38092,14 @@
       <c r="BL184" s="2">
         <v>674</v>
       </c>
+      <c r="BM184" s="2">
+        <v>677</v>
+      </c>
+      <c r="BN184" s="2">
+        <v>680</v>
+      </c>
     </row>
-    <row r="185" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>183</v>
       </c>
@@ -37184,8 +38292,14 @@
       <c r="BL185" s="2">
         <v>643</v>
       </c>
+      <c r="BM185" s="2">
+        <v>663</v>
+      </c>
+      <c r="BN185" s="2">
+        <v>679</v>
+      </c>
     </row>
-    <row r="186" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
         <v>184</v>
       </c>
@@ -37378,8 +38492,14 @@
       <c r="BL186" s="2">
         <v>5367</v>
       </c>
+      <c r="BM186" s="2">
+        <v>5834</v>
+      </c>
+      <c r="BN186" s="2">
+        <v>6276</v>
+      </c>
     </row>
-    <row r="187" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>185</v>
       </c>
@@ -37572,8 +38692,14 @@
       <c r="BL187" s="2">
         <v>326</v>
       </c>
+      <c r="BM187" s="2">
+        <v>331</v>
+      </c>
+      <c r="BN187" s="2">
+        <v>331</v>
+      </c>
     </row>
-    <row r="188" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
         <v>186</v>
       </c>
@@ -37766,8 +38892,14 @@
       <c r="BL188" s="2">
         <v>1136</v>
       </c>
+      <c r="BM188" s="2">
+        <v>1137</v>
+      </c>
+      <c r="BN188" s="2">
+        <v>1137</v>
+      </c>
     </row>
-    <row r="189" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>187</v>
       </c>
@@ -37960,8 +39092,14 @@
       <c r="BL189" s="2">
         <v>1915</v>
       </c>
+      <c r="BM189" s="2">
+        <v>1955</v>
+      </c>
+      <c r="BN189" s="2">
+        <v>1958</v>
+      </c>
     </row>
-    <row r="190" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>188</v>
       </c>
@@ -38154,8 +39292,14 @@
       <c r="BL190" s="2">
         <v>14204</v>
       </c>
+      <c r="BM190" s="2">
+        <v>14792</v>
+      </c>
+      <c r="BN190" s="2">
+        <v>14838</v>
+      </c>
     </row>
-    <row r="191" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
         <v>189</v>
       </c>
@@ -38348,8 +39492,14 @@
       <c r="BL191" s="2">
         <v>133</v>
       </c>
+      <c r="BM191" s="2">
+        <v>133</v>
+      </c>
+      <c r="BN191" s="2">
+        <v>133</v>
+      </c>
     </row>
-    <row r="192" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
         <v>190</v>
       </c>
@@ -38542,8 +39692,14 @@
       <c r="BL192" s="2">
         <v>116</v>
       </c>
+      <c r="BM192" s="2">
+        <v>119</v>
+      </c>
+      <c r="BN192" s="2">
+        <v>119</v>
+      </c>
     </row>
-    <row r="193" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
         <v>191</v>
       </c>
@@ -38736,8 +39892,14 @@
       <c r="BL193" s="2">
         <v>5019</v>
       </c>
+      <c r="BM193" s="2">
+        <v>5159</v>
+      </c>
+      <c r="BN193" s="2">
+        <v>5182</v>
+      </c>
     </row>
-    <row r="194" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>192</v>
       </c>
@@ -38930,8 +40092,14 @@
       <c r="BL194" s="2">
         <v>115</v>
       </c>
+      <c r="BM194" s="2">
+        <v>115</v>
+      </c>
+      <c r="BN194" s="2">
+        <v>115</v>
+      </c>
     </row>
-    <row r="195" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>193</v>
       </c>
@@ -39124,8 +40292,14 @@
       <c r="BL195" s="2">
         <v>139</v>
       </c>
+      <c r="BM195" s="2">
+        <v>140</v>
+      </c>
+      <c r="BN195" s="2">
+        <v>140</v>
+      </c>
     </row>
-    <row r="196" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
         <v>194</v>
       </c>
@@ -39318,8 +40492,14 @@
       <c r="BL196" s="2">
         <v>418</v>
       </c>
+      <c r="BM196" s="2">
+        <v>443</v>
+      </c>
+      <c r="BN196" s="2">
+        <v>456</v>
+      </c>
     </row>
-    <row r="197" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>195</v>
       </c>
@@ -39512,8 +40692,14 @@
       <c r="BL197" s="2">
         <v>235</v>
       </c>
+      <c r="BM197" s="2">
+        <v>239</v>
+      </c>
+      <c r="BN197" s="2">
+        <v>239</v>
+      </c>
     </row>
-    <row r="198" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
         <v>196</v>
       </c>
@@ -39706,8 +40892,14 @@
       <c r="BL198" s="2">
         <v>213</v>
       </c>
+      <c r="BM198" s="2">
+        <v>217</v>
+      </c>
+      <c r="BN198" s="2">
+        <v>223</v>
+      </c>
     </row>
-    <row r="199" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>197</v>
       </c>
@@ -39900,8 +41092,14 @@
       <c r="BL199" s="2">
         <v>7</v>
       </c>
+      <c r="BM199" s="2">
+        <v>7</v>
+      </c>
+      <c r="BN199" s="2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="200" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>198</v>
       </c>
@@ -40094,8 +41292,14 @@
       <c r="BL200" s="2">
         <v>701</v>
       </c>
+      <c r="BM200" s="2">
+        <v>707</v>
+      </c>
+      <c r="BN200" s="2">
+        <v>721</v>
+      </c>
     </row>
-    <row r="201" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
         <v>199</v>
       </c>
@@ -40288,8 +41492,14 @@
       <c r="BL201" s="2">
         <v>4882</v>
       </c>
+      <c r="BM201" s="2">
+        <v>4992</v>
+      </c>
+      <c r="BN201" s="2">
+        <v>5016</v>
+      </c>
     </row>
-    <row r="202" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>200</v>
       </c>
@@ -40482,8 +41692,14 @@
       <c r="BL202" s="2">
         <v>335</v>
       </c>
+      <c r="BM202" s="2">
+        <v>335</v>
+      </c>
+      <c r="BN202" s="2">
+        <v>337</v>
+      </c>
     </row>
-    <row r="203" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
         <v>201</v>
       </c>
@@ -40676,8 +41892,14 @@
       <c r="BL203" s="2">
         <v>1291</v>
       </c>
+      <c r="BM203" s="2">
+        <v>1322</v>
+      </c>
+      <c r="BN203" s="2">
+        <v>1339</v>
+      </c>
     </row>
-    <row r="204" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>202</v>
       </c>
@@ -40870,8 +42092,14 @@
       <c r="BL204" s="2">
         <v>517</v>
       </c>
+      <c r="BM204" s="2">
+        <v>526</v>
+      </c>
+      <c r="BN204" s="2">
+        <v>527</v>
+      </c>
     </row>
-    <row r="205" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A205" s="5" t="s">
         <v>203</v>
       </c>
@@ -41064,8 +42292,14 @@
       <c r="BL205" s="2">
         <v>298</v>
       </c>
+      <c r="BM205" s="2">
+        <v>322</v>
+      </c>
+      <c r="BN205" s="2">
+        <v>347</v>
+      </c>
     </row>
-    <row r="206" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
         <v>204</v>
       </c>
@@ -41258,8 +42492,14 @@
       <c r="BL206" s="2">
         <v>691</v>
       </c>
+      <c r="BM206" s="2">
+        <v>697</v>
+      </c>
+      <c r="BN206" s="2">
+        <v>697</v>
+      </c>
     </row>
-    <row r="207" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
         <v>205</v>
       </c>
@@ -41452,8 +42692,14 @@
       <c r="BL207" s="2">
         <v>1210</v>
       </c>
+      <c r="BM207" s="2">
+        <v>1260</v>
+      </c>
+      <c r="BN207" s="2">
+        <v>1261</v>
+      </c>
     </row>
-    <row r="208" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
         <v>206</v>
       </c>
@@ -41646,8 +42892,14 @@
       <c r="BL208" s="2">
         <v>197</v>
       </c>
+      <c r="BM208" s="2">
+        <v>196</v>
+      </c>
+      <c r="BN208" s="2">
+        <v>196</v>
+      </c>
     </row>
-    <row r="209" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>207</v>
       </c>
@@ -41840,8 +43092,14 @@
       <c r="BL209" s="2">
         <v>106</v>
       </c>
+      <c r="BM209" s="2">
+        <v>107</v>
+      </c>
+      <c r="BN209" s="2">
+        <v>108</v>
+      </c>
     </row>
-    <row r="210" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
         <v>208</v>
       </c>
@@ -42034,8 +43292,14 @@
       <c r="BL210" s="2">
         <v>103</v>
       </c>
+      <c r="BM210" s="2">
+        <v>103</v>
+      </c>
+      <c r="BN210" s="2">
+        <v>103</v>
+      </c>
     </row>
-    <row r="211" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A211" s="5" t="s">
         <v>209</v>
       </c>
@@ -42228,8 +43492,14 @@
       <c r="BL211" s="2">
         <v>44</v>
       </c>
+      <c r="BM211" s="2">
+        <v>44</v>
+      </c>
+      <c r="BN211" s="2">
+        <v>44</v>
+      </c>
     </row>
-    <row r="212" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A212" s="5" t="s">
         <v>210</v>
       </c>
@@ -42422,8 +43692,14 @@
       <c r="BL212" s="2">
         <v>1477</v>
       </c>
+      <c r="BM212" s="2">
+        <v>1504</v>
+      </c>
+      <c r="BN212" s="2">
+        <v>1513</v>
+      </c>
     </row>
-    <row r="213" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A213" s="5" t="s">
         <v>211</v>
       </c>
@@ -42616,8 +43892,14 @@
       <c r="BL213" s="2">
         <v>35</v>
       </c>
+      <c r="BM213" s="2">
+        <v>36</v>
+      </c>
+      <c r="BN213" s="2">
+        <v>36</v>
+      </c>
     </row>
-    <row r="214" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>212</v>
       </c>
@@ -42810,8 +44092,14 @@
       <c r="BL214" s="2">
         <v>7212</v>
       </c>
+      <c r="BM214" s="2">
+        <v>7548</v>
+      </c>
+      <c r="BN214" s="2">
+        <v>7577</v>
+      </c>
     </row>
-    <row r="215" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
         <v>213</v>
       </c>
@@ -43004,8 +44292,14 @@
       <c r="BL215" s="2">
         <v>290</v>
       </c>
+      <c r="BM215" s="2">
+        <v>296</v>
+      </c>
+      <c r="BN215" s="2">
+        <v>299</v>
+      </c>
     </row>
-    <row r="216" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>214</v>
       </c>
@@ -43198,8 +44492,14 @@
       <c r="BL216" s="2">
         <v>2639</v>
       </c>
+      <c r="BM216" s="2">
+        <v>2879</v>
+      </c>
+      <c r="BN216" s="2">
+        <v>2886</v>
+      </c>
     </row>
-    <row r="217" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A217" s="5" t="s">
         <v>215</v>
       </c>
@@ -43392,8 +44692,14 @@
       <c r="BL217" s="2">
         <v>113</v>
       </c>
+      <c r="BM217" s="2">
+        <v>116</v>
+      </c>
+      <c r="BN217" s="2">
+        <v>122</v>
+      </c>
     </row>
-    <row r="218" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A218" s="5" t="s">
         <v>216</v>
       </c>
@@ -43586,8 +44892,14 @@
       <c r="BL218" s="2">
         <v>27</v>
       </c>
+      <c r="BM218" s="2">
+        <v>27</v>
+      </c>
+      <c r="BN218" s="2">
+        <v>27</v>
+      </c>
     </row>
-    <row r="219" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A219" s="5" t="s">
         <v>217</v>
       </c>
@@ -43780,8 +45092,14 @@
       <c r="BL219" s="2">
         <v>9</v>
       </c>
+      <c r="BM219" s="2">
+        <v>9</v>
+      </c>
+      <c r="BN219" s="2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="220" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>218</v>
       </c>
@@ -43974,8 +45292,14 @@
       <c r="BL220" s="2">
         <v>64</v>
       </c>
+      <c r="BM220" s="2">
+        <v>64</v>
+      </c>
+      <c r="BN220" s="2">
+        <v>64</v>
+      </c>
     </row>
-    <row r="221" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
         <v>219</v>
       </c>
@@ -44168,8 +45492,14 @@
       <c r="BL221" s="2">
         <v>254</v>
       </c>
+      <c r="BM221" s="2">
+        <v>257</v>
+      </c>
+      <c r="BN221" s="2">
+        <v>258</v>
+      </c>
     </row>
-    <row r="222" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>220</v>
       </c>
@@ -44362,8 +45692,14 @@
       <c r="BL222" s="2">
         <v>89133</v>
       </c>
+      <c r="BM222" s="2">
+        <v>90269</v>
+      </c>
+      <c r="BN222" s="2">
+        <v>90612</v>
+      </c>
     </row>
-    <row r="223" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A223" s="5" t="s">
         <v>221</v>
       </c>
@@ -44556,8 +45892,14 @@
       <c r="BL223" s="2">
         <v>8087</v>
       </c>
+      <c r="BM223" s="2">
+        <v>8559</v>
+      </c>
+      <c r="BN223" s="2">
+        <v>8671</v>
+      </c>
     </row>
-    <row r="224" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
         <v>222</v>
       </c>
@@ -44750,8 +46092,14 @@
       <c r="BL224" s="2">
         <v>6</v>
       </c>
+      <c r="BM224" s="2">
+        <v>6</v>
+      </c>
+      <c r="BN224" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="225" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A225" s="5" t="s">
         <v>223</v>
       </c>
@@ -44944,8 +46292,14 @@
       <c r="BL225" s="2">
         <v>271</v>
       </c>
+      <c r="BM225" s="2">
+        <v>274</v>
+      </c>
+      <c r="BN225" s="2">
+        <v>282</v>
+      </c>
     </row>
-    <row r="226" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A226" s="5" t="s">
         <v>224</v>
       </c>
@@ -45138,8 +46492,14 @@
       <c r="BL226" s="2">
         <v>43</v>
       </c>
+      <c r="BM226" s="2">
+        <v>43</v>
+      </c>
+      <c r="BN226" s="2">
+        <v>43</v>
+      </c>
     </row>
-    <row r="227" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A227" s="5" t="s">
         <v>225</v>
       </c>
@@ -45332,8 +46692,14 @@
       <c r="BL227" s="2">
         <v>2850</v>
       </c>
+      <c r="BM227" s="2">
+        <v>2916</v>
+      </c>
+      <c r="BN227" s="2">
+        <v>2933</v>
+      </c>
     </row>
-    <row r="228" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A228" s="5" t="s">
         <v>226</v>
       </c>
@@ -45526,8 +46892,14 @@
       <c r="BL228" s="2">
         <v>2731</v>
       </c>
+      <c r="BM228" s="2">
+        <v>2765</v>
+      </c>
+      <c r="BN228" s="2">
+        <v>2784</v>
+      </c>
     </row>
-    <row r="229" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A229" s="5" t="s">
         <v>227</v>
       </c>
@@ -45720,8 +47092,14 @@
       <c r="BL229" s="2">
         <v>56384</v>
       </c>
+      <c r="BM229" s="2">
+        <v>59205</v>
+      </c>
+      <c r="BN229" s="2">
+        <v>60438</v>
+      </c>
     </row>
-    <row r="230" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A230" s="5" t="s">
         <v>228</v>
       </c>
@@ -45914,8 +47292,14 @@
       <c r="BL230" s="2">
         <v>692</v>
       </c>
+      <c r="BM230" s="2">
+        <v>701</v>
+      </c>
+      <c r="BN230" s="2">
+        <v>701</v>
+      </c>
     </row>
-    <row r="231" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A231" s="5" t="s">
         <v>229</v>
       </c>
@@ -46108,8 +47492,14 @@
       <c r="BL231" s="2">
         <v>662</v>
       </c>
+      <c r="BM231" s="2">
+        <v>685</v>
+      </c>
+      <c r="BN231" s="2">
+        <v>695</v>
+      </c>
     </row>
-    <row r="232" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
         <v>230</v>
       </c>
@@ -46302,8 +47692,14 @@
       <c r="BL232" s="2">
         <v>447</v>
       </c>
+      <c r="BM232" s="2">
+        <v>468</v>
+      </c>
+      <c r="BN232" s="2">
+        <v>480</v>
+      </c>
     </row>
-    <row r="233" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A233" s="5" t="s">
         <v>231</v>
       </c>
@@ -46496,8 +47892,14 @@
       <c r="BL233" s="2">
         <v>154</v>
       </c>
+      <c r="BM233" s="2">
+        <v>156</v>
+      </c>
+      <c r="BN233" s="2">
+        <v>157</v>
+      </c>
     </row>
-    <row r="234" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A234" s="5" t="s">
         <v>232</v>
       </c>
@@ -46690,8 +48092,14 @@
       <c r="BL234" s="2">
         <v>895</v>
       </c>
+      <c r="BM234" s="2">
+        <v>938</v>
+      </c>
+      <c r="BN234" s="2">
+        <v>985</v>
+      </c>
     </row>
-    <row r="235" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A235" s="5" t="s">
         <v>233</v>
       </c>
@@ -46884,8 +48292,14 @@
       <c r="BL235" s="2">
         <v>1420</v>
       </c>
+      <c r="BM235" s="2">
+        <v>1523</v>
+      </c>
+      <c r="BN235" s="2">
+        <v>1643</v>
+      </c>
     </row>
-    <row r="236" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A236" s="5" t="s">
         <v>234</v>
       </c>
@@ -47078,8 +48492,14 @@
       <c r="BL236" s="2">
         <v>1484</v>
       </c>
+      <c r="BM236" s="2">
+        <v>1504</v>
+      </c>
+      <c r="BN236" s="2">
+        <v>1509</v>
+      </c>
     </row>
-    <row r="237" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A237" s="5" t="s">
         <v>235</v>
       </c>
@@ -47272,8 +48692,14 @@
       <c r="BL237" s="2">
         <v>3657</v>
       </c>
+      <c r="BM237" s="2">
+        <v>3791</v>
+      </c>
+      <c r="BN237" s="2">
+        <v>3846</v>
+      </c>
     </row>
-    <row r="238" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A238" s="5" t="s">
         <v>236</v>
       </c>
@@ -47466,8 +48892,14 @@
       <c r="BL238" s="2">
         <v>9659</v>
       </c>
+      <c r="BM238" s="2">
+        <v>10649</v>
+      </c>
+      <c r="BN238" s="2">
+        <v>10974</v>
+      </c>
     </row>
-    <row r="239" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A239" s="5" t="s">
         <v>237</v>
       </c>
@@ -47660,8 +49092,14 @@
       <c r="BL239" s="2">
         <v>1769</v>
       </c>
+      <c r="BM239" s="2">
+        <v>1782</v>
+      </c>
+      <c r="BN239" s="2">
+        <v>1786</v>
+      </c>
     </row>
-    <row r="240" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A240" s="5" t="s">
         <v>238</v>
       </c>
@@ -47854,8 +49292,14 @@
       <c r="BL240" s="2">
         <v>249</v>
       </c>
+      <c r="BM240" s="2">
+        <v>250</v>
+      </c>
+      <c r="BN240" s="2">
+        <v>251</v>
+      </c>
     </row>
-    <row r="241" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
         <v>239</v>
       </c>
@@ -48048,8 +49492,14 @@
       <c r="BL241" s="2">
         <v>2484</v>
       </c>
+      <c r="BM241" s="2">
+        <v>2489</v>
+      </c>
+      <c r="BN241" s="2">
+        <v>2510</v>
+      </c>
     </row>
-    <row r="242" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A242" s="5" t="s">
         <v>240</v>
       </c>
@@ -48242,8 +49692,14 @@
       <c r="BL242" s="2">
         <v>8348</v>
       </c>
+      <c r="BM242" s="2">
+        <v>8573</v>
+      </c>
+      <c r="BN242" s="2">
+        <v>8772</v>
+      </c>
     </row>
-    <row r="243" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A243" s="5" t="s">
         <v>241</v>
       </c>
@@ -48436,8 +49892,14 @@
       <c r="BL243" s="2">
         <v>2187</v>
       </c>
+      <c r="BM243" s="2">
+        <v>2248</v>
+      </c>
+      <c r="BN243" s="2">
+        <v>2366</v>
+      </c>
     </row>
-    <row r="244" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A244" s="5" t="s">
         <v>242</v>
       </c>
@@ -48630,8 +50092,14 @@
       <c r="BL244" s="2">
         <v>137</v>
       </c>
+      <c r="BM244" s="2">
+        <v>137</v>
+      </c>
+      <c r="BN244" s="2">
+        <v>137</v>
+      </c>
     </row>
-    <row r="245" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A245" s="5" t="s">
         <v>243</v>
       </c>
@@ -48824,8 +50292,14 @@
       <c r="BL245" s="2">
         <v>6876</v>
       </c>
+      <c r="BM245" s="2">
+        <v>6975</v>
+      </c>
+      <c r="BN245" s="2">
+        <v>6994</v>
+      </c>
     </row>
-    <row r="246" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A246" s="5" t="s">
         <v>244</v>
       </c>
@@ -49018,8 +50492,14 @@
       <c r="BL246" s="2">
         <v>292</v>
       </c>
+      <c r="BM246" s="2">
+        <v>294</v>
+      </c>
+      <c r="BN246" s="2">
+        <v>293</v>
+      </c>
     </row>
-    <row r="247" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A247" s="5" t="s">
         <v>245</v>
       </c>
@@ -49212,8 +50692,14 @@
       <c r="BL247" s="2">
         <v>1635</v>
       </c>
+      <c r="BM247" s="2">
+        <v>1642</v>
+      </c>
+      <c r="BN247" s="2">
+        <v>1645</v>
+      </c>
     </row>
-    <row r="248" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="s">
         <v>246</v>
       </c>
@@ -49406,8 +50892,14 @@
       <c r="BL248" s="2">
         <v>19026</v>
       </c>
+      <c r="BM248" s="2">
+        <v>19687</v>
+      </c>
+      <c r="BN248" s="2">
+        <v>20111</v>
+      </c>
     </row>
-    <row r="249" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A249" s="5" t="s">
         <v>247</v>
       </c>
@@ -49600,8 +51092,14 @@
       <c r="BL249" s="2">
         <v>1213</v>
       </c>
+      <c r="BM249" s="2">
+        <v>1280</v>
+      </c>
+      <c r="BN249" s="2">
+        <v>1325</v>
+      </c>
     </row>
-    <row r="250" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A250" s="5" t="s">
         <v>248</v>
       </c>
@@ -49794,8 +51292,14 @@
       <c r="BL250" s="2">
         <v>35</v>
       </c>
+      <c r="BM250" s="2">
+        <v>35</v>
+      </c>
+      <c r="BN250" s="2">
+        <v>35</v>
+      </c>
     </row>
-    <row r="251" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A251" s="5" t="s">
         <v>249</v>
       </c>
@@ -49988,8 +51492,14 @@
       <c r="BL251" s="2">
         <v>1516</v>
       </c>
+      <c r="BM251" s="2">
+        <v>1527</v>
+      </c>
+      <c r="BN251" s="2">
+        <v>1529</v>
+      </c>
     </row>
-    <row r="252" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A252" s="5" t="s">
         <v>250</v>
       </c>
@@ -50182,8 +51692,14 @@
       <c r="BL252" s="2">
         <v>843</v>
       </c>
+      <c r="BM252" s="2">
+        <v>892</v>
+      </c>
+      <c r="BN252" s="2">
+        <v>904</v>
+      </c>
     </row>
-    <row r="253" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A253" s="5" t="s">
         <v>251</v>
       </c>
@@ -50376,8 +51892,14 @@
       <c r="BL253" s="2">
         <v>221</v>
       </c>
+      <c r="BM253" s="2">
+        <v>226</v>
+      </c>
+      <c r="BN253" s="2">
+        <v>236</v>
+      </c>
     </row>
-    <row r="254" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A254" s="5" t="s">
         <v>252</v>
       </c>
@@ -50570,8 +52092,14 @@
       <c r="BL254" s="2">
         <v>721</v>
       </c>
+      <c r="BM254" s="2">
+        <v>731</v>
+      </c>
+      <c r="BN254" s="2">
+        <v>738</v>
+      </c>
     </row>
-    <row r="255" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A255" s="5" t="s">
         <v>253</v>
       </c>
@@ -50764,8 +52292,14 @@
       <c r="BL255" s="2">
         <v>523</v>
       </c>
+      <c r="BM255" s="2">
+        <v>594</v>
+      </c>
+      <c r="BN255" s="2">
+        <v>594</v>
+      </c>
     </row>
-    <row r="256" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A256" s="5" t="s">
         <v>254</v>
       </c>
@@ -50958,8 +52492,14 @@
       <c r="BL256" s="2">
         <v>126</v>
       </c>
+      <c r="BM256" s="2">
+        <v>126</v>
+      </c>
+      <c r="BN256" s="2">
+        <v>126</v>
+      </c>
     </row>
-    <row r="257" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A257" s="5" t="s">
         <v>255</v>
       </c>
@@ -51152,8 +52692,14 @@
       <c r="BL257" s="2">
         <v>4580</v>
       </c>
+      <c r="BM257" s="2">
+        <v>4586</v>
+      </c>
+      <c r="BN257" s="2">
+        <v>4581</v>
+      </c>
     </row>
-    <row r="258" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A258" s="5" t="s">
         <v>256</v>
       </c>
@@ -51347,8 +52893,14 @@
       <c r="BL258" s="2">
         <v>412201</v>
       </c>
+      <c r="BM258" s="2">
+        <v>414824</v>
+      </c>
+      <c r="BN258" s="2">
+        <v>432152</v>
+      </c>
     </row>
-    <row r="259" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A259" s="9" t="s">
         <v>257</v>
       </c>
@@ -51545,8 +53097,16 @@
       <c r="BL259" s="10">
         <v>1767701</v>
       </c>
+      <c r="BM259" s="10">
+        <f>SUM(BM3:BM258)</f>
+        <v>1805642</v>
+      </c>
+      <c r="BN259" s="10">
+        <f>SUM(BN3:BN258)</f>
+        <v>1836037</v>
+      </c>
     </row>
-    <row r="261" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A261" s="3" t="s">
         <v>261</v>
       </c>
@@ -51559,7 +53119,7 @@
       <c r="H261" s="4"/>
       <c r="I261" s="4"/>
     </row>
-    <row r="262" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:66" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" s="21" t="s">
         <v>258</v>
       </c>
@@ -51572,7 +53132,7 @@
       <c r="H262" s="22"/>
       <c r="I262" s="22"/>
     </row>
-    <row r="263" spans="1:64" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:66" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" s="23" t="s">
         <v>259</v>
       </c>
@@ -51585,7 +53145,7 @@
       <c r="H263" s="24"/>
       <c r="I263" s="24"/>
     </row>
-    <row r="264" spans="1:64" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:66" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" s="23" t="s">
         <v>260</v>
       </c>
@@ -51598,7 +53158,7 @@
       <c r="H264" s="24"/>
       <c r="I264" s="24"/>
     </row>
-    <row r="265" spans="1:64" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:66" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" s="11" t="s">
         <v>288</v>
       </c>
@@ -51660,10 +53220,17 @@
       <c r="BE265" s="13"/>
       <c r="BF265" s="13"/>
       <c r="BG265" s="13"/>
+      <c r="BH265" s="13"/>
+      <c r="BI265" s="13"/>
+      <c r="BJ265" s="13"/>
+      <c r="BK265" s="13"/>
+      <c r="BL265" s="13"/>
+      <c r="BM265" s="13"/>
+      <c r="BN265" s="13"/>
     </row>
-    <row r="266" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:66" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B266" s="18"/>
       <c r="C266" s="13"/>
@@ -51674,7 +53241,7 @@
       <c r="H266" s="13"/>
       <c r="I266" s="13"/>
     </row>
-    <row r="267" spans="1:64" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:66" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" s="23" t="s">
         <v>278</v>
       </c>

</xml_diff>